<commit_message>
fix bug identified by John Burns in documentation of AUTOPF/autopsyresultsavailable
</commit_message>
<xml_diff>
--- a/input/images/IJE_File_Layouts_Version_2021_FHIR.xlsx
+++ b/input/images/IJE_File_Layouts_Version_2021_FHIR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skravitz/git/vrdr/input/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E211C6DE-E5FA-4D44-BE8B-A15A873C5868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BFFEBC1-0B34-9145-A323-EF97A8F81967}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6620" yWindow="500" windowWidth="60640" windowHeight="23560" tabRatio="779" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7716" uniqueCount="2670">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7716" uniqueCount="2671">
   <si>
     <t>u</t>
   </si>
@@ -9262,6 +9262,9 @@
   </si>
   <si>
     <t>REPLACE (*deprecated*)</t>
+  </si>
+  <si>
+    <t>component[ autopsyResultsAvailable ].value</t>
   </si>
 </sst>
 </file>
@@ -11851,8 +11854,8 @@
   </sheetPr>
   <dimension ref="A1:L283"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A201" zoomScale="170" zoomScaleNormal="170" zoomScaleSheetLayoutView="95" workbookViewId="0">
-      <selection activeCell="E204" sqref="E204"/>
+    <sheetView tabSelected="1" topLeftCell="A111" zoomScale="170" zoomScaleNormal="170" zoomScaleSheetLayoutView="95" workbookViewId="0">
+      <selection activeCell="I126" sqref="I126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13"/>
@@ -16314,7 +16317,7 @@
         <v>2384</v>
       </c>
       <c r="I126" s="7" t="s">
-        <v>2599</v>
+        <v>2670</v>
       </c>
       <c r="J126" s="16" t="s">
         <v>2361</v>

</xml_diff>

<commit_message>
added PartialDateTime to PPTIME
</commit_message>
<xml_diff>
--- a/input/images/IJE_File_Layouts_Version_2021_FHIR.xlsx
+++ b/input/images/IJE_File_Layouts_Version_2021_FHIR.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skravitz/git/vrdr/input/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BFFEBC1-0B34-9145-A323-EF97A8F81967}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{565C296E-0C05-E34C-8B57-BE4F8DEA08E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6620" yWindow="500" windowWidth="60640" windowHeight="23560" tabRatio="779" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11854,8 +11854,8 @@
   </sheetPr>
   <dimension ref="A1:L283"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" zoomScale="170" zoomScaleNormal="170" zoomScaleSheetLayoutView="95" workbookViewId="0">
-      <selection activeCell="I126" sqref="I126"/>
+    <sheetView tabSelected="1" topLeftCell="A104" zoomScale="170" zoomScaleNormal="170" zoomScaleSheetLayoutView="95" workbookViewId="0">
+      <selection activeCell="K104" sqref="K104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13"/>
@@ -20253,8 +20253,8 @@
       <c r="J238" s="16" t="s">
         <v>2332</v>
       </c>
-      <c r="K238" s="7" t="s">
-        <v>2595</v>
+      <c r="K238" s="16" t="s">
+        <v>2453</v>
       </c>
     </row>
     <row r="239" spans="1:12" ht="14">
@@ -67895,7 +67895,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -68102,12 +68107,7 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -68117,9 +68117,9 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6E1C13E-614F-4B48-A9FE-F6158F0F568F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2D8D0BD-9993-4EC8-86D1-0A7C5F6E1934}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -68144,9 +68144,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2D8D0BD-9993-4EC8-86D1-0A7C5F6E1934}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6E1C13E-614F-4B48-A9FE-F6158F0F568F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
delete example that caused trouble, along with suppressed warnings, and add spreadsheet
</commit_message>
<xml_diff>
--- a/input/images/IJE_File_Layouts_Version_2021_FHIR.xlsx
+++ b/input/images/IJE_File_Layouts_Version_2021_FHIR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skravitz/git/vrdr/input/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{565C296E-0C05-E34C-8B57-BE4F8DEA08E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2438A77-2022-534F-BB52-99A0B2D63A02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6620" yWindow="500" windowWidth="60640" windowHeight="23560" tabRatio="779" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11854,8 +11854,8 @@
   </sheetPr>
   <dimension ref="A1:L283"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A104" zoomScale="170" zoomScaleNormal="170" zoomScaleSheetLayoutView="95" workbookViewId="0">
-      <selection activeCell="K104" sqref="K104"/>
+    <sheetView tabSelected="1" topLeftCell="A236" zoomScale="170" zoomScaleNormal="170" zoomScaleSheetLayoutView="95" workbookViewId="0">
+      <selection activeCell="K239" sqref="K239"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13"/>
@@ -20289,8 +20289,8 @@
       <c r="J239" s="16" t="s">
         <v>2332</v>
       </c>
-      <c r="K239" s="7" t="s">
-        <v>2595</v>
+      <c r="K239" s="16" t="s">
+        <v>2453</v>
       </c>
     </row>
     <row r="240" spans="1:12" ht="14">

</xml_diff>

<commit_message>
fix new warnings/errors from IGP...groan
</commit_message>
<xml_diff>
--- a/input/images/IJE_File_Layouts_Version_2021_FHIR.xlsx
+++ b/input/images/IJE_File_Layouts_Version_2021_FHIR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skravitz/git/vrdr/input/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2438A77-2022-534F-BB52-99A0B2D63A02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4B5AD72-53BF-2F44-B762-A8F581D40942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6620" yWindow="500" windowWidth="60640" windowHeight="23560" tabRatio="779" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11855,7 +11855,7 @@
   <dimension ref="A1:L283"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A236" zoomScale="170" zoomScaleNormal="170" zoomScaleSheetLayoutView="95" workbookViewId="0">
-      <selection activeCell="K239" sqref="K239"/>
+      <selection activeCell="I238" sqref="I238"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13"/>

</xml_diff>

<commit_message>
Fixed documentation on First/Second Native American Race literal
</commit_message>
<xml_diff>
--- a/input/images/IJE_File_Layouts_Version_2021_FHIR.xlsx
+++ b/input/images/IJE_File_Layouts_Version_2021_FHIR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skravitz/git/vrdr/input/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE5B4B3F-5DB3-2C45-BA7F-9C4C78D37B19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AC0A68E-DFEA-4C4F-B571-4B916FB366AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6620" yWindow="500" windowWidth="60640" windowHeight="23560" tabRatio="779" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7716" uniqueCount="2676">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7716" uniqueCount="2678">
   <si>
     <t>u</t>
   </si>
@@ -9280,6 +9280,12 @@
   </si>
   <si>
     <t>component[ SecondOtherRaceLiteral].valueString</t>
+  </si>
+  <si>
+    <t>component[ FirstAmericanIndianorAlaskanNativeLiteral].valueString</t>
+  </si>
+  <si>
+    <t>component[ SecondAmericanIndianorAlaskanNativeLiteral].valueString</t>
   </si>
 </sst>
 </file>
@@ -11870,7 +11876,7 @@
   <dimension ref="A1:L283"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A65" zoomScale="170" zoomScaleNormal="170" zoomScaleSheetLayoutView="95" workbookViewId="0">
-      <selection activeCell="I79" sqref="I79"/>
+      <selection activeCell="E67" sqref="E67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13"/>
@@ -14428,7 +14434,7 @@
         <v>2493</v>
       </c>
       <c r="I71" s="16" t="s">
-        <v>2514</v>
+        <v>2676</v>
       </c>
       <c r="J71" s="16" t="s">
         <v>2322</v>
@@ -14466,7 +14472,7 @@
         <v>2493</v>
       </c>
       <c r="I72" s="16" t="s">
-        <v>2515</v>
+        <v>2677</v>
       </c>
       <c r="J72" s="16" t="s">
         <v>2322</v>
@@ -18050,7 +18056,7 @@
         <v>2575</v>
       </c>
     </row>
-    <row r="176" spans="1:12" ht="28">
+    <row r="176" spans="1:12" ht="14">
       <c r="A176" s="15">
         <f t="shared" si="7"/>
         <v>156</v>
@@ -19701,7 +19707,7 @@
         <v>2325</v>
       </c>
     </row>
-    <row r="223" spans="1:12" ht="28">
+    <row r="223" spans="1:12" ht="14">
       <c r="A223" s="15">
         <f t="shared" si="10"/>
         <v>203</v>
@@ -67910,7 +67916,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -68117,12 +68128,7 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -68132,9 +68138,9 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6E1C13E-614F-4B48-A9FE-F6158F0F568F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2D8D0BD-9993-4EC8-86D1-0A7C5F6E1934}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -68159,9 +68165,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2D8D0BD-9993-4EC8-86D1-0A7C5F6E1934}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6E1C13E-614F-4B48-A9FE-F6158F0F568F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
make the ppdatetime a time or datetime to handle case where data is absent
</commit_message>
<xml_diff>
--- a/input/images/IJE_File_Layouts_Version_2021_FHIR.xlsx
+++ b/input/images/IJE_File_Layouts_Version_2021_FHIR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skravitz/git/vrdr/input/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AC0A68E-DFEA-4C4F-B571-4B916FB366AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E37594D-0792-7A4D-8BE3-8688AADB5049}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6620" yWindow="500" windowWidth="60640" windowHeight="23560" tabRatio="779" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7716" uniqueCount="2678">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7714" uniqueCount="2681">
   <si>
     <t>u</t>
   </si>
@@ -9282,10 +9282,19 @@
     <t>component[ SecondOtherRaceLiteral].valueString</t>
   </si>
   <si>
-    <t>component[ FirstAmericanIndianorAlaskanNativeLiteral].valueString</t>
-  </si>
-  <si>
-    <t>component[ SecondAmericanIndianorAlaskanNativeLiteral].valueString</t>
+    <t>component[ FirstAmericanIndianOrAlaskanNativeLiteral].valueString</t>
+  </si>
+  <si>
+    <t>component[ SecondAmericanIndianOrAlaskanNativeLiteral].valueString</t>
+  </si>
+  <si>
+    <t>component[datetimePronouncedDead].valueDateTime if a date is also specified, or component[datetimePronouncedDead].valueTime if no date is specified</t>
+  </si>
+  <si>
+    <t>component[datetimePronouncedDead	].valueDateTime</t>
+  </si>
+  <si>
+    <t>dateTime or time</t>
   </si>
 </sst>
 </file>
@@ -11875,8 +11884,8 @@
   </sheetPr>
   <dimension ref="A1:L283"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="170" zoomScaleNormal="170" zoomScaleSheetLayoutView="95" workbookViewId="0">
-      <selection activeCell="E67" sqref="E67"/>
+    <sheetView tabSelected="1" topLeftCell="A236" zoomScale="170" zoomScaleNormal="170" zoomScaleSheetLayoutView="95" workbookViewId="0">
+      <selection activeCell="K239" sqref="K239"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13"/>
@@ -20269,14 +20278,12 @@
         <v>2407</v>
       </c>
       <c r="I238" s="16" t="s">
-        <v>2597</v>
+        <v>2679</v>
       </c>
       <c r="J238" s="16" t="s">
         <v>2332</v>
       </c>
-      <c r="K238" s="16" t="s">
-        <v>2453</v>
-      </c>
+      <c r="K238" s="16"/>
     </row>
     <row r="239" spans="1:12" ht="14">
       <c r="A239" s="15">
@@ -20305,14 +20312,12 @@
         <v>2407</v>
       </c>
       <c r="I239" s="16" t="s">
-        <v>2598</v>
+        <v>2678</v>
       </c>
       <c r="J239" s="16" t="s">
-        <v>2332</v>
-      </c>
-      <c r="K239" s="16" t="s">
-        <v>2453</v>
-      </c>
+        <v>2680</v>
+      </c>
+      <c r="K239" s="16"/>
     </row>
     <row r="240" spans="1:12" ht="14">
       <c r="A240" s="15">
@@ -21765,7 +21770,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{440A4221-87BC-6346-98ED-4929CFD2A733}">
-  <sheetPr>
+  <sheetPr codeName="Sheet5">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:L168"/>
@@ -42811,7 +42816,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Sheet6">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:G376"/>
@@ -50384,6 +50389,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:G169"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -53857,7 +53863,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Sheet8">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:IE368"/>

</xml_diff>

<commit_message>
fix PacificIsland --> PacificIslander
</commit_message>
<xml_diff>
--- a/input/images/IJE_File_Layouts_Version_2021_FHIR.xlsx
+++ b/input/images/IJE_File_Layouts_Version_2021_FHIR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skravitz/git/vrdr/input/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE5B4B3F-5DB3-2C45-BA7F-9C4C78D37B19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{941E4845-F21D-FB4C-ABEE-C3258303671A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6620" yWindow="500" windowWidth="60640" windowHeight="23560" tabRatio="779" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7716" uniqueCount="2676">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7716" uniqueCount="2677">
   <si>
     <t>u</t>
   </si>
@@ -9273,13 +9273,16 @@
     <t>component[ SecondOtherAsianLiteral].valueString</t>
   </si>
   <si>
-    <t>component[ FirstOtherPacificIslandLiteral].valueString</t>
-  </si>
-  <si>
     <t>component[ FirstOtherRaceLiteral].valueString</t>
   </si>
   <si>
     <t>component[ SecondOtherRaceLiteral].valueString</t>
+  </si>
+  <si>
+    <t>component[ FirstOtherPacificIslanderLiteral].valueString</t>
+  </si>
+  <si>
+    <t>component[ SecondOtherPacificIslanderLiteral].valueString</t>
   </si>
 </sst>
 </file>
@@ -11869,8 +11872,8 @@
   </sheetPr>
   <dimension ref="A1:L283"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="170" zoomScaleNormal="170" zoomScaleSheetLayoutView="95" workbookViewId="0">
-      <selection activeCell="I79" sqref="I79"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="170" zoomScaleNormal="170" zoomScaleSheetLayoutView="95" workbookViewId="0">
+      <selection activeCell="I76" sqref="I76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13"/>
@@ -14580,7 +14583,7 @@
         <v>2493</v>
       </c>
       <c r="I75" s="16" t="s">
-        <v>2673</v>
+        <v>2675</v>
       </c>
       <c r="J75" s="16" t="s">
         <v>2322</v>
@@ -14618,7 +14621,7 @@
         <v>2493</v>
       </c>
       <c r="I76" s="16" t="s">
-        <v>2673</v>
+        <v>2676</v>
       </c>
       <c r="J76" s="16" t="s">
         <v>2322</v>
@@ -14656,7 +14659,7 @@
         <v>2493</v>
       </c>
       <c r="I77" s="16" t="s">
-        <v>2674</v>
+        <v>2673</v>
       </c>
       <c r="J77" s="16" t="s">
         <v>2322</v>
@@ -14694,7 +14697,7 @@
         <v>2493</v>
       </c>
       <c r="I78" s="16" t="s">
-        <v>2675</v>
+        <v>2674</v>
       </c>
       <c r="J78" s="16" t="s">
         <v>2322</v>
@@ -18050,7 +18053,7 @@
         <v>2575</v>
       </c>
     </row>
-    <row r="176" spans="1:12" ht="28">
+    <row r="176" spans="1:12" ht="14">
       <c r="A176" s="15">
         <f t="shared" si="7"/>
         <v>156</v>
@@ -19701,7 +19704,7 @@
         <v>2325</v>
       </c>
     </row>
-    <row r="223" spans="1:12" ht="28">
+    <row r="223" spans="1:12" ht="14">
       <c r="A223" s="15">
         <f t="shared" si="10"/>
         <v>203</v>
@@ -67910,10 +67913,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002752A2C1F044FE469AAF2142AB326B8C" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c07487fc32f7ac2d3b3707e982dea906">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c1a58edb-1ba6-4800-9942-1e1defaa36d6" xmlns:ns3="4b113022-9134-4b2e-abe8-26e86c9e296e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="be9eaf82d0c074f79785b0acc776d2a9" ns2:_="" ns3:_="">
     <xsd:import namespace="c1a58edb-1ba6-4800-9942-1e1defaa36d6"/>
@@ -68116,30 +68130,36 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6E1C13E-614F-4B48-A9FE-F6158F0F568F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4A36FDD-FA0C-40EF-989B-74F1F7876F18}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="4b113022-9134-4b2e-abe8-26e86c9e296e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="c1a58edb-1ba6-4800-9942-1e1defaa36d6"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2D8D0BD-9993-4EC8-86D1-0A7C5F6E1934}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D3F3134-699E-462F-8D9F-EA7A8DE51B1D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -68158,27 +68178,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2D8D0BD-9993-4EC8-86D1-0A7C5F6E1934}">
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6E1C13E-614F-4B48-A9FE-F6158F0F568F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4A36FDD-FA0C-40EF-989B-74F1F7876F18}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="4b113022-9134-4b2e-abe8-26e86c9e296e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="c1a58edb-1ba6-4800-9942-1e1defaa36d6"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Finish cause of death part 1
</commit_message>
<xml_diff>
--- a/input/images/IJE_File_Layouts_Version_2021_FHIR.xlsx
+++ b/input/images/IJE_File_Layouts_Version_2021_FHIR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skravitz/git/vrdr/input/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{827D0C9B-C939-BC4B-9F5F-12445651310C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDE65E62-66F0-064B-99F2-5321AFA74CC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6620" yWindow="500" windowWidth="60640" windowHeight="23560" tabRatio="779" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7716" uniqueCount="2677">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7714" uniqueCount="2688">
   <si>
     <t>u</t>
   </si>
@@ -9284,6 +9284,39 @@
   <si>
     <t>component[ SecondOtherPacificIslanderLiteral].valueString</t>
   </si>
+  <si>
+    <t>component[interval].valueString or component[interval].valueQuantity , component[lineNumber] = 1</t>
+  </si>
+  <si>
+    <t>component[interval].valueString or component[interval].valueQuantity, component[lineNumber] = 2</t>
+  </si>
+  <si>
+    <t>component[interval].valueString or component[interval].valueQuantity, component[lineNumber] = 3</t>
+  </si>
+  <si>
+    <t>component[interval].valueString or component[interval].valueQuantity, component[lineNumber] = 4</t>
+  </si>
+  <si>
+    <t>string(20), or Quantity</t>
+  </si>
+  <si>
+    <t>Note: Quantity not yet supported for NCHS Submissions.   [UnitsOfAgeVS]</t>
+  </si>
+  <si>
+    <t>component[datetimePronouncedDead ].valueDateTime</t>
+  </si>
+  <si>
+    <t>dateTime or Time</t>
+  </si>
+  <si>
+    <t>component[datetimePronouncedDead].valueDateTime if a date is also specified, or component[datetimePronouncedDead].valueTime if no date is specified</t>
+  </si>
+  <si>
+    <t>component[ FirstAmericanIndianOrAlaskanNativeLiteral].valueString</t>
+  </si>
+  <si>
+    <t>component[ SecondAmericanIndianOrAlaskanNativeLiteral].valueString</t>
+  </si>
 </sst>
 </file>
 
@@ -9292,7 +9325,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="36">
+  <fonts count="37">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -9493,6 +9526,12 @@
     </font>
     <font>
       <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -9919,7 +9958,7 @@
     <xf numFmtId="164" fontId="19" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="367">
+  <cellXfs count="368">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -10969,6 +11008,9 @@
     <xf numFmtId="0" fontId="14" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -11872,8 +11914,8 @@
   </sheetPr>
   <dimension ref="A1:L283"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="170" zoomScaleNormal="170" zoomScaleSheetLayoutView="95" workbookViewId="0">
-      <selection activeCell="I76" sqref="I76"/>
+    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="170" zoomScaleNormal="170" zoomScaleSheetLayoutView="95" workbookViewId="0">
+      <selection activeCell="I73" sqref="I73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13"/>
@@ -12802,7 +12844,7 @@
       <c r="J28" s="16" t="s">
         <v>2361</v>
       </c>
-      <c r="K28" s="7" t="s">
+      <c r="K28" s="16" t="s">
         <v>2404</v>
       </c>
       <c r="L28" s="7" t="s">
@@ -14431,7 +14473,7 @@
         <v>2493</v>
       </c>
       <c r="I71" s="16" t="s">
-        <v>2514</v>
+        <v>2686</v>
       </c>
       <c r="J71" s="16" t="s">
         <v>2322</v>
@@ -14469,7 +14511,7 @@
         <v>2493</v>
       </c>
       <c r="I72" s="16" t="s">
-        <v>2515</v>
+        <v>2687</v>
       </c>
       <c r="J72" s="16" t="s">
         <v>2322</v>
@@ -19115,14 +19157,14 @@
       <c r="H206" s="16" t="s">
         <v>2378</v>
       </c>
-      <c r="I206" s="7" t="s">
-        <v>2609</v>
+      <c r="I206" s="16" t="s">
+        <v>2677</v>
       </c>
       <c r="J206" s="16" t="s">
-        <v>2382</v>
-      </c>
-      <c r="K206" s="7" t="s">
-        <v>2595</v>
+        <v>2681</v>
+      </c>
+      <c r="K206" s="16" t="s">
+        <v>2682</v>
       </c>
       <c r="L206" s="7" t="s">
         <v>2575</v>
@@ -19191,14 +19233,14 @@
       <c r="H208" s="16" t="s">
         <v>2378</v>
       </c>
-      <c r="I208" s="7" t="s">
-        <v>2614</v>
+      <c r="I208" s="16" t="s">
+        <v>2678</v>
       </c>
       <c r="J208" s="16" t="s">
-        <v>2382</v>
-      </c>
-      <c r="K208" s="7" t="s">
-        <v>2595</v>
+        <v>2681</v>
+      </c>
+      <c r="K208" s="16" t="s">
+        <v>2682</v>
       </c>
       <c r="L208" s="7" t="s">
         <v>2575</v>
@@ -19267,14 +19309,14 @@
       <c r="H210" s="16" t="s">
         <v>2378</v>
       </c>
-      <c r="I210" s="7" t="s">
-        <v>2612</v>
+      <c r="I210" s="16" t="s">
+        <v>2679</v>
       </c>
       <c r="J210" s="16" t="s">
-        <v>2382</v>
-      </c>
-      <c r="K210" s="7" t="s">
-        <v>2595</v>
+        <v>2681</v>
+      </c>
+      <c r="K210" s="16" t="s">
+        <v>2682</v>
       </c>
       <c r="L210" s="7" t="s">
         <v>2575</v>
@@ -19343,14 +19385,14 @@
       <c r="H212" s="16" t="s">
         <v>2378</v>
       </c>
-      <c r="I212" s="7" t="s">
-        <v>2610</v>
+      <c r="I212" s="16" t="s">
+        <v>2680</v>
       </c>
       <c r="J212" s="16" t="s">
-        <v>2382</v>
-      </c>
-      <c r="K212" s="7" t="s">
-        <v>2595</v>
+        <v>2681</v>
+      </c>
+      <c r="K212" s="16" t="s">
+        <v>2682</v>
       </c>
       <c r="L212" s="7" t="s">
         <v>2575</v>
@@ -20266,16 +20308,14 @@
         <v>2407</v>
       </c>
       <c r="I238" s="16" t="s">
-        <v>2597</v>
+        <v>2683</v>
       </c>
       <c r="J238" s="16" t="s">
         <v>2332</v>
       </c>
-      <c r="K238" s="16" t="s">
-        <v>2453</v>
-      </c>
-    </row>
-    <row r="239" spans="1:12" ht="14">
+      <c r="K238" s="16"/>
+    </row>
+    <row r="239" spans="1:12" ht="56">
       <c r="A239" s="15">
         <f t="shared" si="10"/>
         <v>219</v>
@@ -20301,15 +20341,13 @@
       <c r="H239" s="16" t="s">
         <v>2407</v>
       </c>
-      <c r="I239" s="16" t="s">
-        <v>2598</v>
+      <c r="I239" s="367" t="s">
+        <v>2685</v>
       </c>
       <c r="J239" s="16" t="s">
-        <v>2332</v>
-      </c>
-      <c r="K239" s="16" t="s">
-        <v>2453</v>
-      </c>
+        <v>2684</v>
+      </c>
+      <c r="K239" s="16"/>
     </row>
     <row r="240" spans="1:12" ht="14">
       <c r="A240" s="15">
@@ -67913,21 +67951,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002752A2C1F044FE469AAF2142AB326B8C" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c07487fc32f7ac2d3b3707e982dea906">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c1a58edb-1ba6-4800-9942-1e1defaa36d6" xmlns:ns3="4b113022-9134-4b2e-abe8-26e86c9e296e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="be9eaf82d0c074f79785b0acc776d2a9" ns2:_="" ns3:_="">
     <xsd:import namespace="c1a58edb-1ba6-4800-9942-1e1defaa36d6"/>
@@ -68130,36 +68153,26 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4A36FDD-FA0C-40EF-989B-74F1F7876F18}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="4b113022-9134-4b2e-abe8-26e86c9e296e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="c1a58edb-1ba6-4800-9942-1e1defaa36d6"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2D8D0BD-9993-4EC8-86D1-0A7C5F6E1934}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D3F3134-699E-462F-8D9F-EA7A8DE51B1D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -68178,6 +68191,31 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2D8D0BD-9993-4EC8-86D1-0A7C5F6E1934}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4A36FDD-FA0C-40EF-989B-74F1F7876F18}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="4b113022-9134-4b2e-abe8-26e86c9e296e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="c1a58edb-1ba6-4800-9942-1e1defaa36d6"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6E1C13E-614F-4B48-A9FE-F6158F0F568F}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
more tweaks to narrative to get links to work
</commit_message>
<xml_diff>
--- a/input/images/IJE_File_Layouts_Version_2021_FHIR.xlsx
+++ b/input/images/IJE_File_Layouts_Version_2021_FHIR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skravitz/git/vrdr/input/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12D8A055-3A88-8B47-8B2D-296BF4C33667}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A5DB007-9B48-3244-B908-82ECF43CF877}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19280" yWindow="5200" windowWidth="30240" windowHeight="18880" tabRatio="779" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11616,7 +11616,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="56">
+    <row r="38" spans="1:7" ht="70">
       <c r="A38" s="78">
         <v>40029</v>
       </c>
@@ -11708,7 +11708,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="140">
+    <row r="49" spans="1:2" ht="154">
       <c r="A49" s="59">
         <v>39867</v>
       </c>
@@ -18091,7 +18091,7 @@
         <v>2575</v>
       </c>
     </row>
-    <row r="177" spans="1:12" ht="14">
+    <row r="177" spans="1:12" ht="28">
       <c r="A177" s="15">
         <f t="shared" si="7"/>
         <v>156</v>
@@ -19742,7 +19742,7 @@
         <v>2325</v>
       </c>
     </row>
-    <row r="224" spans="1:12" ht="14">
+    <row r="224" spans="1:12" ht="28">
       <c r="A224" s="15">
         <f t="shared" si="10"/>
         <v>203</v>
@@ -27781,7 +27781,7 @@
   <dimension ref="A1:N258"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="95" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13"/>
@@ -28003,7 +28003,7 @@
         <v>2322</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>2684</v>
+        <v>2687</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="14">
@@ -28035,7 +28035,7 @@
         <v>2322</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>2684</v>
+        <v>2687</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="14">
@@ -28067,7 +28067,7 @@
         <v>2322</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>2684</v>
+        <v>2687</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="27" customHeight="1">
@@ -32046,7 +32046,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="14">
+    <row r="64" spans="1:6" ht="28">
       <c r="A64" s="18">
         <v>55</v>
       </c>
@@ -46981,7 +46981,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="209" spans="1:6" ht="14">
+    <row r="209" spans="1:6" ht="28">
       <c r="A209" s="132">
         <v>201</v>
       </c>
@@ -55597,7 +55597,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="14">
+    <row r="65" spans="1:6" ht="28">
       <c r="A65" s="18">
         <v>55</v>
       </c>
@@ -67977,12 +67977,7 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -68189,7 +68184,12 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -68199,9 +68199,9 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2D8D0BD-9993-4EC8-86D1-0A7C5F6E1934}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6E1C13E-614F-4B48-A9FE-F6158F0F568F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -68226,9 +68226,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6E1C13E-614F-4B48-A9FE-F6158F0F568F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2D8D0BD-9993-4EC8-86D1-0A7C5F6E1934}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
fix COUNTYC and CITYC types in data dictionary and some typos
</commit_message>
<xml_diff>
--- a/input/images/IJE_File_Layouts_Version_2021_FHIR.xlsx
+++ b/input/images/IJE_File_Layouts_Version_2021_FHIR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skravitz/git/vrdr/input/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A5DB007-9B48-3244-B908-82ECF43CF877}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8C62024-E97C-1444-9563-CF670A55B3CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19280" yWindow="5200" windowWidth="30240" windowHeight="18880" tabRatio="779" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4000" yWindow="500" windowWidth="63620" windowHeight="27760" tabRatio="779" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Frontpage" sheetId="7" r:id="rId1"/>
@@ -25,6 +25,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Mortality!$A$5:$L$280</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Mortality Roster'!$B$7:$K$255</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Natality!$A$8:$IE$367</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Surveillance!$A$5:$L$164</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="7">'Birth Infant Death'!$A$1:$F$368</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="5">'Fetal Death'!$A$1:$F$376</definedName>
@@ -11616,7 +11617,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="70">
+    <row r="38" spans="1:7" ht="56">
       <c r="A38" s="78">
         <v>40029</v>
       </c>
@@ -11700,7 +11701,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="154">
+    <row r="48" spans="1:7" ht="140">
       <c r="A48" s="59">
         <v>39887</v>
       </c>
@@ -11708,7 +11709,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="154">
+    <row r="49" spans="1:2" ht="140">
       <c r="A49" s="59">
         <v>39867</v>
       </c>
@@ -11875,8 +11876,8 @@
   </sheetPr>
   <dimension ref="A1:L284"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScale="170" zoomScaleNormal="170" zoomScaleSheetLayoutView="95" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="G39" zoomScale="220" zoomScaleNormal="220" zoomScaleSheetLayoutView="95" workbookViewId="0">
+      <selection activeCell="K37" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13"/>
@@ -13142,7 +13143,7 @@
         <v>2600</v>
       </c>
       <c r="J37" s="16" t="s">
-        <v>2322</v>
+        <v>2320</v>
       </c>
       <c r="K37" s="7" t="s">
         <v>2454</v>
@@ -13180,7 +13181,7 @@
         <v>2601</v>
       </c>
       <c r="J38" s="16" t="s">
-        <v>2322</v>
+        <v>2320</v>
       </c>
       <c r="K38" s="16" t="s">
         <v>2455</v>
@@ -27780,8 +27781,8 @@
   </sheetPr>
   <dimension ref="A1:N258"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="95" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView topLeftCell="C11" zoomScale="160" zoomScaleNormal="160" zoomScaleSheetLayoutView="95" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14:F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13"/>
@@ -30379,13 +30380,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <sheetPr codeName="Sheet4">
+  <sheetPr codeName="Sheet4" filterMode="1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:IE369"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView zoomScale="230" zoomScaleNormal="230" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13"/>
@@ -30960,7 +30961,7 @@
       <c r="ID8"/>
       <c r="IE8"/>
     </row>
-    <row r="9" spans="1:239" ht="15" customHeight="1" thickBot="1">
+    <row r="9" spans="1:239" ht="15" hidden="1" customHeight="1" thickBot="1">
       <c r="A9" s="329" t="s">
         <v>60</v>
       </c>
@@ -30970,7 +30971,7 @@
       <c r="E9" s="329"/>
       <c r="F9" s="330"/>
     </row>
-    <row r="10" spans="1:239" ht="14">
+    <row r="10" spans="1:239" ht="14" hidden="1">
       <c r="A10" s="18">
         <v>1</v>
       </c>
@@ -30990,7 +30991,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:239" ht="293">
+    <row r="11" spans="1:239" ht="293" hidden="1">
       <c r="A11" s="18">
         <v>2</v>
       </c>
@@ -31010,7 +31011,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="12" spans="1:239" ht="14">
+    <row r="12" spans="1:239" ht="14" hidden="1">
       <c r="A12" s="18">
         <v>3</v>
       </c>
@@ -31030,7 +31031,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="13" spans="1:239" ht="28">
+    <row r="13" spans="1:239" ht="28" hidden="1">
       <c r="A13" s="18">
         <v>4</v>
       </c>
@@ -31050,7 +31051,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="14" spans="1:239" ht="14">
+    <row r="14" spans="1:239" ht="14" hidden="1">
       <c r="A14" s="18">
         <v>5</v>
       </c>
@@ -31070,7 +31071,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="15" spans="1:239" ht="14">
+    <row r="15" spans="1:239" ht="14" hidden="1">
       <c r="A15" s="18">
         <v>6</v>
       </c>
@@ -31090,7 +31091,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="16" spans="1:239" ht="42">
+    <row r="16" spans="1:239" ht="42" hidden="1">
       <c r="A16" s="18">
         <v>7</v>
       </c>
@@ -31110,7 +31111,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="14">
+    <row r="17" spans="1:6" ht="14" hidden="1">
       <c r="A17" s="18">
         <v>8</v>
       </c>
@@ -31130,7 +31131,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="14">
+    <row r="18" spans="1:6" ht="14" hidden="1">
       <c r="A18" s="18">
         <v>9</v>
       </c>
@@ -31170,7 +31171,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="112">
+    <row r="20" spans="1:6" ht="112" hidden="1">
       <c r="A20" s="18">
         <v>11</v>
       </c>
@@ -31190,7 +31191,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="14">
+    <row r="21" spans="1:6" ht="14" hidden="1">
       <c r="A21" s="18">
         <v>12</v>
       </c>
@@ -31208,7 +31209,7 @@
       </c>
       <c r="F21" s="96"/>
     </row>
-    <row r="22" spans="1:6" ht="14">
+    <row r="22" spans="1:6" ht="14" hidden="1">
       <c r="A22" s="18">
         <v>13</v>
       </c>
@@ -31226,7 +31227,7 @@
       </c>
       <c r="F22" s="93"/>
     </row>
-    <row r="23" spans="1:6" ht="14">
+    <row r="23" spans="1:6" ht="14" hidden="1">
       <c r="A23" s="18">
         <v>14</v>
       </c>
@@ -31246,7 +31247,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="14">
+    <row r="24" spans="1:6" ht="14" hidden="1">
       <c r="A24" s="18">
         <v>15</v>
       </c>
@@ -31266,7 +31267,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="14">
+    <row r="25" spans="1:6" ht="14" hidden="1">
       <c r="A25" s="18">
         <v>16</v>
       </c>
@@ -31286,7 +31287,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="28">
+    <row r="26" spans="1:6" ht="28" hidden="1">
       <c r="A26" s="18">
         <v>17</v>
       </c>
@@ -31306,7 +31307,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="345">
+    <row r="27" spans="1:6" ht="345" hidden="1">
       <c r="A27" s="18">
         <v>18</v>
       </c>
@@ -31326,7 +31327,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="14">
+    <row r="28" spans="1:6" ht="14" hidden="1">
       <c r="A28" s="18">
         <v>19</v>
       </c>
@@ -31346,7 +31347,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="14">
+    <row r="29" spans="1:6" ht="14" hidden="1">
       <c r="A29" s="18">
         <v>20</v>
       </c>
@@ -31386,7 +31387,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="345">
+    <row r="31" spans="1:6" ht="345" hidden="1">
       <c r="A31" s="18">
         <v>22</v>
       </c>
@@ -31406,7 +31407,7 @@
         <v>790</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="14">
+    <row r="32" spans="1:6" ht="14" hidden="1">
       <c r="A32" s="18">
         <v>23</v>
       </c>
@@ -31426,7 +31427,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="42">
+    <row r="33" spans="1:6" ht="42" hidden="1">
       <c r="A33" s="18">
         <v>24</v>
       </c>
@@ -31446,7 +31447,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="14">
+    <row r="34" spans="1:6" ht="14" hidden="1">
       <c r="A34" s="18">
         <v>25</v>
       </c>
@@ -31466,7 +31467,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="14">
+    <row r="35" spans="1:6" ht="14" hidden="1">
       <c r="A35" s="18">
         <v>26</v>
       </c>
@@ -31486,7 +31487,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="14">
+    <row r="36" spans="1:6" ht="14" hidden="1">
       <c r="A36" s="18">
         <v>27</v>
       </c>
@@ -31506,7 +31507,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="28">
+    <row r="37" spans="1:6" ht="28" hidden="1">
       <c r="A37" s="18">
         <v>28</v>
       </c>
@@ -31526,7 +31527,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="42">
+    <row r="38" spans="1:6" ht="42" hidden="1">
       <c r="A38" s="18">
         <v>29</v>
       </c>
@@ -31546,7 +31547,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="42">
+    <row r="39" spans="1:6" ht="42" hidden="1">
       <c r="A39" s="18">
         <v>30</v>
       </c>
@@ -31566,7 +31567,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="56">
+    <row r="40" spans="1:6" ht="56" hidden="1">
       <c r="A40" s="18">
         <v>31</v>
       </c>
@@ -31586,7 +31587,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="126">
+    <row r="41" spans="1:6" ht="126" hidden="1">
       <c r="A41" s="18">
         <v>32</v>
       </c>
@@ -31606,7 +31607,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="42">
+    <row r="42" spans="1:6" ht="42" hidden="1">
       <c r="A42" s="18">
         <v>33</v>
       </c>
@@ -31626,7 +31627,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="42">
+    <row r="43" spans="1:6" ht="42" hidden="1">
       <c r="A43" s="18">
         <v>34</v>
       </c>
@@ -31646,7 +31647,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="42">
+    <row r="44" spans="1:6" ht="42" hidden="1">
       <c r="A44" s="18">
         <v>35</v>
       </c>
@@ -31666,7 +31667,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="42">
+    <row r="45" spans="1:6" ht="42" hidden="1">
       <c r="A45" s="18">
         <v>36</v>
       </c>
@@ -31686,7 +31687,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="42">
+    <row r="46" spans="1:6" ht="42" hidden="1">
       <c r="A46" s="18">
         <v>37</v>
       </c>
@@ -31706,7 +31707,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="14">
+    <row r="47" spans="1:6" ht="14" hidden="1">
       <c r="A47" s="18">
         <v>38</v>
       </c>
@@ -31726,7 +31727,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="28">
+    <row r="48" spans="1:6" ht="28" hidden="1">
       <c r="A48" s="18">
         <v>39</v>
       </c>
@@ -31746,7 +31747,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="14">
+    <row r="49" spans="1:6" ht="14" hidden="1">
       <c r="A49" s="18">
         <v>40</v>
       </c>
@@ -31766,7 +31767,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="14">
+    <row r="50" spans="1:6" ht="14" hidden="1">
       <c r="A50" s="18">
         <v>41</v>
       </c>
@@ -31786,7 +31787,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="14">
+    <row r="51" spans="1:6" ht="14" hidden="1">
       <c r="A51" s="18">
         <v>42</v>
       </c>
@@ -31806,7 +31807,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="14">
+    <row r="52" spans="1:6" ht="14" hidden="1">
       <c r="A52" s="18">
         <v>43</v>
       </c>
@@ -31826,7 +31827,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="14">
+    <row r="53" spans="1:6" ht="14" hidden="1">
       <c r="A53" s="18">
         <v>44</v>
       </c>
@@ -31846,7 +31847,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="14">
+    <row r="54" spans="1:6" ht="14" hidden="1">
       <c r="A54" s="18">
         <v>45</v>
       </c>
@@ -31866,7 +31867,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="14">
+    <row r="55" spans="1:6" ht="14" hidden="1">
       <c r="A55" s="18">
         <v>46</v>
       </c>
@@ -31886,7 +31887,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="14">
+    <row r="56" spans="1:6" ht="14" hidden="1">
       <c r="A56" s="18">
         <v>47</v>
       </c>
@@ -31906,7 +31907,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="14">
+    <row r="57" spans="1:6" ht="14" hidden="1">
       <c r="A57" s="18">
         <v>48</v>
       </c>
@@ -31926,7 +31927,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="14">
+    <row r="58" spans="1:6" ht="14" hidden="1">
       <c r="A58" s="18">
         <v>49</v>
       </c>
@@ -31946,7 +31947,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="14">
+    <row r="59" spans="1:6" ht="14" hidden="1">
       <c r="A59" s="18">
         <v>50</v>
       </c>
@@ -31966,7 +31967,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="14">
+    <row r="60" spans="1:6" ht="14" hidden="1">
       <c r="A60" s="18">
         <v>51</v>
       </c>
@@ -31986,7 +31987,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="14">
+    <row r="61" spans="1:6" ht="14" hidden="1">
       <c r="A61" s="18">
         <v>52</v>
       </c>
@@ -32006,7 +32007,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="14">
+    <row r="62" spans="1:6" ht="14" hidden="1">
       <c r="A62" s="18">
         <v>53</v>
       </c>
@@ -32026,7 +32027,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="14">
+    <row r="63" spans="1:6" ht="14" hidden="1">
       <c r="A63" s="18">
         <v>54</v>
       </c>
@@ -32046,7 +32047,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="28">
+    <row r="64" spans="1:6" ht="28" hidden="1">
       <c r="A64" s="18">
         <v>55</v>
       </c>
@@ -32066,7 +32067,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="14">
+    <row r="65" spans="1:6" ht="14" hidden="1">
       <c r="A65" s="18">
         <v>56</v>
       </c>
@@ -32086,7 +32087,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="14">
+    <row r="66" spans="1:6" ht="14" hidden="1">
       <c r="A66" s="18">
         <v>57</v>
       </c>
@@ -32106,7 +32107,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="14">
+    <row r="67" spans="1:6" ht="14" hidden="1">
       <c r="A67" s="18">
         <v>58</v>
       </c>
@@ -32126,7 +32127,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="14">
+    <row r="68" spans="1:6" ht="14" hidden="1">
       <c r="A68" s="18">
         <v>59</v>
       </c>
@@ -32146,7 +32147,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="14">
+    <row r="69" spans="1:6" ht="14" hidden="1">
       <c r="A69" s="18">
         <v>60</v>
       </c>
@@ -32166,7 +32167,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="14">
+    <row r="70" spans="1:6" ht="14" hidden="1">
       <c r="A70" s="18">
         <v>61</v>
       </c>
@@ -32186,7 +32187,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="27" customHeight="1">
+    <row r="71" spans="1:6" ht="27" hidden="1" customHeight="1">
       <c r="A71" s="18">
         <v>62</v>
       </c>
@@ -32206,7 +32207,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="72" spans="1:6">
+    <row r="72" spans="1:6" hidden="1">
       <c r="A72" s="18">
         <v>63</v>
       </c>
@@ -32226,7 +32227,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="73" spans="1:6">
+    <row r="73" spans="1:6" hidden="1">
       <c r="A73" s="18">
         <v>64</v>
       </c>
@@ -32246,7 +32247,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="74" spans="1:6">
+    <row r="74" spans="1:6" hidden="1">
       <c r="A74" s="18">
         <v>65</v>
       </c>
@@ -32266,7 +32267,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="75" spans="1:6">
+    <row r="75" spans="1:6" hidden="1">
       <c r="A75" s="18">
         <v>66</v>
       </c>
@@ -32286,7 +32287,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="76" spans="1:6">
+    <row r="76" spans="1:6" hidden="1">
       <c r="A76" s="18">
         <v>67</v>
       </c>
@@ -32306,7 +32307,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="77" spans="1:6">
+    <row r="77" spans="1:6" hidden="1">
       <c r="A77" s="18">
         <v>68</v>
       </c>
@@ -32326,7 +32327,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="78" spans="1:6">
+    <row r="78" spans="1:6" hidden="1">
       <c r="A78" s="18">
         <v>69</v>
       </c>
@@ -32346,7 +32347,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="79" spans="1:6">
+    <row r="79" spans="1:6" hidden="1">
       <c r="A79" s="18">
         <v>70</v>
       </c>
@@ -32366,7 +32367,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="80" spans="1:6">
+    <row r="80" spans="1:6" hidden="1">
       <c r="A80" s="18">
         <v>71</v>
       </c>
@@ -32386,7 +32387,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="81" spans="1:6">
+    <row r="81" spans="1:6" hidden="1">
       <c r="A81" s="18">
         <v>72</v>
       </c>
@@ -32406,7 +32407,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="82" spans="1:6">
+    <row r="82" spans="1:6" hidden="1">
       <c r="A82" s="18">
         <v>73</v>
       </c>
@@ -32426,7 +32427,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="83" spans="1:6">
+    <row r="83" spans="1:6" hidden="1">
       <c r="A83" s="18">
         <v>74</v>
       </c>
@@ -32446,7 +32447,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="84" spans="1:6">
+    <row r="84" spans="1:6" hidden="1">
       <c r="A84" s="18">
         <v>75</v>
       </c>
@@ -32466,7 +32467,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="85" spans="1:6">
+    <row r="85" spans="1:6" hidden="1">
       <c r="A85" s="18">
         <v>76</v>
       </c>
@@ -32486,7 +32487,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="86" spans="1:6">
+    <row r="86" spans="1:6" hidden="1">
       <c r="A86" s="18">
         <v>77</v>
       </c>
@@ -32506,7 +32507,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="126">
+    <row r="87" spans="1:6" ht="126" hidden="1">
       <c r="A87" s="18">
         <v>78</v>
       </c>
@@ -32526,7 +32527,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="42">
+    <row r="88" spans="1:6" ht="42" hidden="1">
       <c r="A88" s="18">
         <v>79</v>
       </c>
@@ -32546,7 +32547,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="42">
+    <row r="89" spans="1:6" ht="42" hidden="1">
       <c r="A89" s="18">
         <v>80</v>
       </c>
@@ -32566,7 +32567,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="42">
+    <row r="90" spans="1:6" ht="42" hidden="1">
       <c r="A90" s="18">
         <v>81</v>
       </c>
@@ -32586,7 +32587,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="42">
+    <row r="91" spans="1:6" ht="42" hidden="1">
       <c r="A91" s="18">
         <v>82</v>
       </c>
@@ -32606,7 +32607,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="42">
+    <row r="92" spans="1:6" ht="42" hidden="1">
       <c r="A92" s="18">
         <v>83</v>
       </c>
@@ -32626,7 +32627,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="93" spans="1:6" ht="14">
+    <row r="93" spans="1:6" ht="14" hidden="1">
       <c r="A93" s="18">
         <v>84</v>
       </c>
@@ -32646,7 +32647,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="94" spans="1:6" ht="28">
+    <row r="94" spans="1:6" ht="28" hidden="1">
       <c r="A94" s="18">
         <v>85</v>
       </c>
@@ -32666,7 +32667,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="95" spans="1:6" ht="14">
+    <row r="95" spans="1:6" ht="14" hidden="1">
       <c r="A95" s="18">
         <v>86</v>
       </c>
@@ -32686,7 +32687,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="96" spans="1:6" ht="12" customHeight="1">
+    <row r="96" spans="1:6" ht="12" hidden="1" customHeight="1">
       <c r="A96" s="18">
         <v>87</v>
       </c>
@@ -32706,7 +32707,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="97" spans="1:6" ht="14">
+    <row r="97" spans="1:6" ht="14" hidden="1">
       <c r="A97" s="18">
         <v>88</v>
       </c>
@@ -32726,7 +32727,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="98" spans="1:6" ht="14">
+    <row r="98" spans="1:6" ht="14" hidden="1">
       <c r="A98" s="18">
         <v>89</v>
       </c>
@@ -32746,7 +32747,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="99" spans="1:6" ht="14">
+    <row r="99" spans="1:6" ht="14" hidden="1">
       <c r="A99" s="18">
         <v>90</v>
       </c>
@@ -32766,7 +32767,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="100" spans="1:6" ht="14">
+    <row r="100" spans="1:6" ht="14" hidden="1">
       <c r="A100" s="18">
         <v>91</v>
       </c>
@@ -32786,7 +32787,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="101" spans="1:6" ht="14">
+    <row r="101" spans="1:6" ht="14" hidden="1">
       <c r="A101" s="18">
         <v>92</v>
       </c>
@@ -32806,7 +32807,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="102" spans="1:6" ht="14">
+    <row r="102" spans="1:6" ht="14" hidden="1">
       <c r="A102" s="18">
         <v>93</v>
       </c>
@@ -32826,7 +32827,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="103" spans="1:6" ht="14">
+    <row r="103" spans="1:6" ht="14" hidden="1">
       <c r="A103" s="18">
         <v>94</v>
       </c>
@@ -32846,7 +32847,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="104" spans="1:6" ht="14">
+    <row r="104" spans="1:6" ht="14" hidden="1">
       <c r="A104" s="18">
         <v>95</v>
       </c>
@@ -32866,7 +32867,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="105" spans="1:6" ht="14">
+    <row r="105" spans="1:6" ht="14" hidden="1">
       <c r="A105" s="18">
         <v>96</v>
       </c>
@@ -32886,7 +32887,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="106" spans="1:6" ht="14">
+    <row r="106" spans="1:6" ht="14" hidden="1">
       <c r="A106" s="18">
         <v>97</v>
       </c>
@@ -32906,7 +32907,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="107" spans="1:6" ht="14">
+    <row r="107" spans="1:6" ht="14" hidden="1">
       <c r="A107" s="18">
         <v>98</v>
       </c>
@@ -32926,7 +32927,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="108" spans="1:6" ht="14">
+    <row r="108" spans="1:6" ht="14" hidden="1">
       <c r="A108" s="18">
         <v>99</v>
       </c>
@@ -32946,7 +32947,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="109" spans="1:6" ht="14">
+    <row r="109" spans="1:6" ht="14" hidden="1">
       <c r="A109" s="18">
         <v>100</v>
       </c>
@@ -32966,7 +32967,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="110" spans="1:6" ht="14">
+    <row r="110" spans="1:6" ht="14" hidden="1">
       <c r="A110" s="18">
         <v>101</v>
       </c>
@@ -32986,7 +32987,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="111" spans="1:6" ht="14">
+    <row r="111" spans="1:6" ht="14" hidden="1">
       <c r="A111" s="18">
         <v>102</v>
       </c>
@@ -33006,7 +33007,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="112" spans="1:6" ht="14">
+    <row r="112" spans="1:6" ht="14" hidden="1">
       <c r="A112" s="18">
         <v>103</v>
       </c>
@@ -33026,7 +33027,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="113" spans="1:6" ht="14">
+    <row r="113" spans="1:6" ht="14" hidden="1">
       <c r="A113" s="18">
         <v>104</v>
       </c>
@@ -33046,7 +33047,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="114" spans="1:6" ht="14">
+    <row r="114" spans="1:6" ht="14" hidden="1">
       <c r="A114" s="18">
         <v>105</v>
       </c>
@@ -33066,7 +33067,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="115" spans="1:6" ht="14">
+    <row r="115" spans="1:6" ht="14" hidden="1">
       <c r="A115" s="18">
         <v>106</v>
       </c>
@@ -33086,7 +33087,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="116" spans="1:6" ht="14">
+    <row r="116" spans="1:6" ht="14" hidden="1">
       <c r="A116" s="18">
         <v>107</v>
       </c>
@@ -33106,7 +33107,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="117" spans="1:6" ht="27.75" customHeight="1">
+    <row r="117" spans="1:6" ht="27.75" hidden="1" customHeight="1">
       <c r="A117" s="18">
         <v>108</v>
       </c>
@@ -33126,7 +33127,7 @@
         <v>1014</v>
       </c>
     </row>
-    <row r="118" spans="1:6">
+    <row r="118" spans="1:6" hidden="1">
       <c r="A118" s="18">
         <v>109</v>
       </c>
@@ -33146,7 +33147,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="119" spans="1:6">
+    <row r="119" spans="1:6" hidden="1">
       <c r="A119" s="18">
         <v>110</v>
       </c>
@@ -33166,7 +33167,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="120" spans="1:6">
+    <row r="120" spans="1:6" hidden="1">
       <c r="A120" s="18">
         <v>111</v>
       </c>
@@ -33186,7 +33187,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="121" spans="1:6">
+    <row r="121" spans="1:6" hidden="1">
       <c r="A121" s="18">
         <v>112</v>
       </c>
@@ -33206,7 +33207,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="122" spans="1:6">
+    <row r="122" spans="1:6" hidden="1">
       <c r="A122" s="18">
         <v>113</v>
       </c>
@@ -33226,7 +33227,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="123" spans="1:6">
+    <row r="123" spans="1:6" hidden="1">
       <c r="A123" s="18">
         <v>114</v>
       </c>
@@ -33246,7 +33247,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="124" spans="1:6">
+    <row r="124" spans="1:6" hidden="1">
       <c r="A124" s="18">
         <v>115</v>
       </c>
@@ -33266,7 +33267,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="125" spans="1:6">
+    <row r="125" spans="1:6" hidden="1">
       <c r="A125" s="18">
         <v>116</v>
       </c>
@@ -33286,7 +33287,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="126" spans="1:6">
+    <row r="126" spans="1:6" hidden="1">
       <c r="A126" s="18">
         <v>117</v>
       </c>
@@ -33306,7 +33307,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="127" spans="1:6">
+    <row r="127" spans="1:6" hidden="1">
       <c r="A127" s="18">
         <v>118</v>
       </c>
@@ -33326,7 +33327,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="128" spans="1:6">
+    <row r="128" spans="1:6" hidden="1">
       <c r="A128" s="18">
         <v>119</v>
       </c>
@@ -33346,7 +33347,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="129" spans="1:6">
+    <row r="129" spans="1:6" hidden="1">
       <c r="A129" s="18">
         <v>120</v>
       </c>
@@ -33366,7 +33367,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="130" spans="1:6">
+    <row r="130" spans="1:6" hidden="1">
       <c r="A130" s="18">
         <v>121</v>
       </c>
@@ -33386,7 +33387,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="131" spans="1:6">
+    <row r="131" spans="1:6" hidden="1">
       <c r="A131" s="18">
         <v>122</v>
       </c>
@@ -33406,7 +33407,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="132" spans="1:6">
+    <row r="132" spans="1:6" hidden="1">
       <c r="A132" s="18">
         <v>123</v>
       </c>
@@ -33426,7 +33427,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="133" spans="1:6" ht="84">
+    <row r="133" spans="1:6" ht="84" hidden="1">
       <c r="A133" s="18">
         <v>124</v>
       </c>
@@ -33446,7 +33447,7 @@
         <v>1048</v>
       </c>
     </row>
-    <row r="134" spans="1:6" ht="42">
+    <row r="134" spans="1:6" ht="42" hidden="1">
       <c r="A134" s="18">
         <v>125</v>
       </c>
@@ -33466,7 +33467,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="135" spans="1:6" ht="14">
+    <row r="135" spans="1:6" ht="14" hidden="1">
       <c r="A135" s="18">
         <v>126</v>
       </c>
@@ -33486,7 +33487,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="136" spans="1:6" ht="14">
+    <row r="136" spans="1:6" ht="14" hidden="1">
       <c r="A136" s="18">
         <v>127</v>
       </c>
@@ -33506,7 +33507,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="137" spans="1:6" ht="24.75" customHeight="1">
+    <row r="137" spans="1:6" ht="24.75" hidden="1" customHeight="1">
       <c r="A137" s="18">
         <v>128</v>
       </c>
@@ -33526,7 +33527,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="138" spans="1:6" ht="28">
+    <row r="138" spans="1:6" ht="28" hidden="1">
       <c r="A138" s="18">
         <v>129</v>
       </c>
@@ -33546,7 +33547,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="139" spans="1:6" ht="28">
+    <row r="139" spans="1:6" ht="28" hidden="1">
       <c r="A139" s="18">
         <v>130</v>
       </c>
@@ -33566,7 +33567,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="140" spans="1:6" ht="28">
+    <row r="140" spans="1:6" ht="28" hidden="1">
       <c r="A140" s="18">
         <v>131</v>
       </c>
@@ -33586,7 +33587,7 @@
         <v>1067</v>
       </c>
     </row>
-    <row r="141" spans="1:6" ht="14">
+    <row r="141" spans="1:6" ht="14" hidden="1">
       <c r="A141" s="18">
         <v>132</v>
       </c>
@@ -33606,7 +33607,7 @@
         <v>1070</v>
       </c>
     </row>
-    <row r="142" spans="1:6" ht="42">
+    <row r="142" spans="1:6" ht="42" hidden="1">
       <c r="A142" s="18">
         <v>133</v>
       </c>
@@ -33626,7 +33627,7 @@
         <v>1074</v>
       </c>
     </row>
-    <row r="143" spans="1:6" ht="14">
+    <row r="143" spans="1:6" ht="14" hidden="1">
       <c r="A143" s="18">
         <v>134</v>
       </c>
@@ -33646,7 +33647,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="144" spans="1:6" ht="14">
+    <row r="144" spans="1:6" ht="14" hidden="1">
       <c r="A144" s="18">
         <v>135</v>
       </c>
@@ -33666,7 +33667,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="145" spans="1:6" ht="42">
+    <row r="145" spans="1:6" ht="42" hidden="1">
       <c r="A145" s="18">
         <v>136</v>
       </c>
@@ -33686,7 +33687,7 @@
         <v>1074</v>
       </c>
     </row>
-    <row r="146" spans="1:6" ht="14">
+    <row r="146" spans="1:6" ht="14" hidden="1">
       <c r="A146" s="18">
         <v>137</v>
       </c>
@@ -33706,7 +33707,7 @@
         <v>1087</v>
       </c>
     </row>
-    <row r="147" spans="1:6" ht="42">
+    <row r="147" spans="1:6" ht="42" hidden="1">
       <c r="A147" s="18">
         <v>138</v>
       </c>
@@ -33726,7 +33727,7 @@
         <v>1074</v>
       </c>
     </row>
-    <row r="148" spans="1:6" ht="14">
+    <row r="148" spans="1:6" ht="14" hidden="1">
       <c r="A148" s="18">
         <v>139</v>
       </c>
@@ -33746,7 +33747,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="149" spans="1:6" ht="42">
+    <row r="149" spans="1:6" ht="42" hidden="1">
       <c r="A149" s="18">
         <v>140</v>
       </c>
@@ -33766,7 +33767,7 @@
         <v>1074</v>
       </c>
     </row>
-    <row r="150" spans="1:6" ht="42">
+    <row r="150" spans="1:6" ht="42" hidden="1">
       <c r="A150" s="18">
         <v>141</v>
       </c>
@@ -33786,7 +33787,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="151" spans="1:6" ht="14">
+    <row r="151" spans="1:6" ht="14" hidden="1">
       <c r="A151" s="18">
         <v>142</v>
       </c>
@@ -33806,7 +33807,7 @@
         <v>1102</v>
       </c>
     </row>
-    <row r="152" spans="1:6" ht="14">
+    <row r="152" spans="1:6" ht="14" hidden="1">
       <c r="A152" s="18">
         <v>143</v>
       </c>
@@ -33826,7 +33827,7 @@
         <v>1102</v>
       </c>
     </row>
-    <row r="153" spans="1:6" ht="14">
+    <row r="153" spans="1:6" ht="14" hidden="1">
       <c r="A153" s="18">
         <v>144</v>
       </c>
@@ -33846,7 +33847,7 @@
         <v>1102</v>
       </c>
     </row>
-    <row r="154" spans="1:6" ht="14">
+    <row r="154" spans="1:6" ht="14" hidden="1">
       <c r="A154" s="18">
         <v>145</v>
       </c>
@@ -33866,7 +33867,7 @@
         <v>1109</v>
       </c>
     </row>
-    <row r="155" spans="1:6" ht="28">
+    <row r="155" spans="1:6" ht="28" hidden="1">
       <c r="A155" s="18">
         <v>146</v>
       </c>
@@ -33886,7 +33887,7 @@
         <v>1112</v>
       </c>
     </row>
-    <row r="156" spans="1:6" ht="14">
+    <row r="156" spans="1:6" ht="14" hidden="1">
       <c r="A156" s="18">
         <v>147</v>
       </c>
@@ -33906,7 +33907,7 @@
         <v>1109</v>
       </c>
     </row>
-    <row r="157" spans="1:6" ht="28">
+    <row r="157" spans="1:6" ht="28" hidden="1">
       <c r="A157" s="18">
         <v>148</v>
       </c>
@@ -33926,7 +33927,7 @@
         <v>1112</v>
       </c>
     </row>
-    <row r="158" spans="1:6" ht="14">
+    <row r="158" spans="1:6" ht="14" hidden="1">
       <c r="A158" s="18">
         <v>149</v>
       </c>
@@ -33946,7 +33947,7 @@
         <v>1070</v>
       </c>
     </row>
-    <row r="159" spans="1:6" ht="14">
+    <row r="159" spans="1:6" ht="14" hidden="1">
       <c r="A159" s="18">
         <v>150</v>
       </c>
@@ -33966,7 +33967,7 @@
         <v>1070</v>
       </c>
     </row>
-    <row r="160" spans="1:6" ht="14">
+    <row r="160" spans="1:6" ht="14" hidden="1">
       <c r="A160" s="18">
         <v>151</v>
       </c>
@@ -33986,7 +33987,7 @@
         <v>1070</v>
       </c>
     </row>
-    <row r="161" spans="1:6" ht="14">
+    <row r="161" spans="1:6" ht="14" hidden="1">
       <c r="A161" s="18">
         <v>152</v>
       </c>
@@ -34006,7 +34007,7 @@
         <v>1070</v>
       </c>
     </row>
-    <row r="162" spans="1:6" ht="112">
+    <row r="162" spans="1:6" ht="112" hidden="1">
       <c r="A162" s="18">
         <v>153</v>
       </c>
@@ -34026,7 +34027,7 @@
         <v>1128</v>
       </c>
     </row>
-    <row r="163" spans="1:6" ht="42">
+    <row r="163" spans="1:6" ht="42" hidden="1">
       <c r="A163" s="18">
         <v>154</v>
       </c>
@@ -34046,7 +34047,7 @@
         <v>1131</v>
       </c>
     </row>
-    <row r="164" spans="1:6" ht="14">
+    <row r="164" spans="1:6" ht="14" hidden="1">
       <c r="A164" s="18">
         <v>155</v>
       </c>
@@ -34066,7 +34067,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="165" spans="1:6" ht="14">
+    <row r="165" spans="1:6" ht="14" hidden="1">
       <c r="A165" s="18">
         <v>156</v>
       </c>
@@ -34086,7 +34087,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="166" spans="1:6" ht="42">
+    <row r="166" spans="1:6" ht="42" hidden="1">
       <c r="A166" s="18">
         <v>157</v>
       </c>
@@ -34106,7 +34107,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="167" spans="1:6" ht="14">
+    <row r="167" spans="1:6" ht="14" hidden="1">
       <c r="A167" s="18">
         <v>158</v>
       </c>
@@ -34126,7 +34127,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="168" spans="1:6" ht="14">
+    <row r="168" spans="1:6" ht="14" hidden="1">
       <c r="A168" s="18">
         <v>159</v>
       </c>
@@ -34146,7 +34147,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="169" spans="1:6" ht="28">
+    <row r="169" spans="1:6" ht="28" hidden="1">
       <c r="A169" s="18">
         <v>160</v>
       </c>
@@ -34166,7 +34167,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="170" spans="1:6" ht="14">
+    <row r="170" spans="1:6" ht="14" hidden="1">
       <c r="A170" s="18">
         <v>161</v>
       </c>
@@ -34186,7 +34187,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="171" spans="1:6" ht="28">
+    <row r="171" spans="1:6" ht="28" hidden="1">
       <c r="A171" s="18">
         <v>162</v>
       </c>
@@ -34206,7 +34207,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="172" spans="1:6" ht="28">
+    <row r="172" spans="1:6" ht="28" hidden="1">
       <c r="A172" s="18">
         <v>163</v>
       </c>
@@ -34226,7 +34227,7 @@
         <v>1158</v>
       </c>
     </row>
-    <row r="173" spans="1:6" ht="28">
+    <row r="173" spans="1:6" ht="28" hidden="1">
       <c r="A173" s="18">
         <v>164</v>
       </c>
@@ -34246,7 +34247,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="174" spans="1:6" ht="14">
+    <row r="174" spans="1:6" ht="14" hidden="1">
       <c r="A174" s="18">
         <v>165</v>
       </c>
@@ -34266,7 +34267,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="175" spans="1:6" ht="14">
+    <row r="175" spans="1:6" ht="14" hidden="1">
       <c r="A175" s="18">
         <v>166</v>
       </c>
@@ -34286,7 +34287,7 @@
         <v>1102</v>
       </c>
     </row>
-    <row r="176" spans="1:6" ht="28">
+    <row r="176" spans="1:6" ht="28" hidden="1">
       <c r="A176" s="18">
         <v>167</v>
       </c>
@@ -34306,7 +34307,7 @@
         <v>1170</v>
       </c>
     </row>
-    <row r="177" spans="1:6" ht="42">
+    <row r="177" spans="1:6" ht="42" hidden="1">
       <c r="A177" s="18">
         <v>168</v>
       </c>
@@ -34326,7 +34327,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="178" spans="1:6" ht="14">
+    <row r="178" spans="1:6" ht="14" hidden="1">
       <c r="A178" s="18">
         <v>169</v>
       </c>
@@ -34346,7 +34347,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="179" spans="1:6" ht="28">
+    <row r="179" spans="1:6" ht="28" hidden="1">
       <c r="A179" s="18">
         <v>170</v>
       </c>
@@ -34366,7 +34367,7 @@
         <v>1158</v>
       </c>
     </row>
-    <row r="180" spans="1:6" ht="14">
+    <row r="180" spans="1:6" ht="14" hidden="1">
       <c r="A180" s="18">
         <v>171</v>
       </c>
@@ -34386,7 +34387,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="181" spans="1:6" ht="14">
+    <row r="181" spans="1:6" ht="14" hidden="1">
       <c r="A181" s="18">
         <v>172</v>
       </c>
@@ -34406,7 +34407,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="182" spans="1:6" ht="14">
+    <row r="182" spans="1:6" ht="14" hidden="1">
       <c r="A182" s="18">
         <v>173</v>
       </c>
@@ -34426,7 +34427,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="183" spans="1:6" ht="42">
+    <row r="183" spans="1:6" ht="42" hidden="1">
       <c r="A183" s="18">
         <v>174</v>
       </c>
@@ -34446,7 +34447,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="184" spans="1:6" ht="28">
+    <row r="184" spans="1:6" ht="28" hidden="1">
       <c r="A184" s="18">
         <v>175</v>
       </c>
@@ -34466,7 +34467,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="185" spans="1:6" ht="14">
+    <row r="185" spans="1:6" ht="14" hidden="1">
       <c r="A185" s="18">
         <v>176</v>
       </c>
@@ -34486,7 +34487,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="186" spans="1:6" ht="14">
+    <row r="186" spans="1:6" ht="14" hidden="1">
       <c r="A186" s="18">
         <v>177</v>
       </c>
@@ -34506,7 +34507,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="187" spans="1:6" ht="42">
+    <row r="187" spans="1:6" ht="42" hidden="1">
       <c r="A187" s="18">
         <v>178</v>
       </c>
@@ -34526,7 +34527,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="188" spans="1:6" ht="28">
+    <row r="188" spans="1:6" ht="28" hidden="1">
       <c r="A188" s="18">
         <v>179</v>
       </c>
@@ -34546,7 +34547,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="189" spans="1:6" ht="28">
+    <row r="189" spans="1:6" ht="28" hidden="1">
       <c r="A189" s="18">
         <v>180</v>
       </c>
@@ -34566,7 +34567,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="190" spans="1:6" ht="42">
+    <row r="190" spans="1:6" ht="42" hidden="1">
       <c r="A190" s="18">
         <v>181</v>
       </c>
@@ -34586,7 +34587,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="191" spans="1:6" ht="14">
+    <row r="191" spans="1:6" ht="14" hidden="1">
       <c r="A191" s="18">
         <v>182</v>
       </c>
@@ -34606,7 +34607,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="192" spans="1:6" ht="30.75" customHeight="1">
+    <row r="192" spans="1:6" ht="30.75" hidden="1" customHeight="1">
       <c r="A192" s="18">
         <v>183</v>
       </c>
@@ -34626,7 +34627,7 @@
         <v>1158</v>
       </c>
     </row>
-    <row r="193" spans="1:6" ht="14">
+    <row r="193" spans="1:6" ht="14" hidden="1">
       <c r="A193" s="18">
         <v>184</v>
       </c>
@@ -34646,7 +34647,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="194" spans="1:6" ht="14">
+    <row r="194" spans="1:6" ht="14" hidden="1">
       <c r="A194" s="18">
         <v>185</v>
       </c>
@@ -34666,7 +34667,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="195" spans="1:6" ht="14">
+    <row r="195" spans="1:6" ht="14" hidden="1">
       <c r="A195" s="18">
         <v>186</v>
       </c>
@@ -34686,7 +34687,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="196" spans="1:6" ht="28">
+    <row r="196" spans="1:6" ht="28" hidden="1">
       <c r="A196" s="18">
         <v>187</v>
       </c>
@@ -34706,7 +34707,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="197" spans="1:6" ht="28">
+    <row r="197" spans="1:6" ht="28" hidden="1">
       <c r="A197" s="18">
         <v>188</v>
       </c>
@@ -34726,7 +34727,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="198" spans="1:6" ht="14">
+    <row r="198" spans="1:6" ht="14" hidden="1">
       <c r="A198" s="18">
         <v>189</v>
       </c>
@@ -34746,7 +34747,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="199" spans="1:6" ht="28">
+    <row r="199" spans="1:6" ht="28" hidden="1">
       <c r="A199" s="18">
         <v>190</v>
       </c>
@@ -34766,7 +34767,7 @@
         <v>1158</v>
       </c>
     </row>
-    <row r="200" spans="1:6" ht="28">
+    <row r="200" spans="1:6" ht="28" hidden="1">
       <c r="A200" s="18">
         <v>191</v>
       </c>
@@ -34786,7 +34787,7 @@
         <v>1158</v>
       </c>
     </row>
-    <row r="201" spans="1:6" ht="56">
+    <row r="201" spans="1:6" ht="56" hidden="1">
       <c r="A201" s="18">
         <v>192</v>
       </c>
@@ -34806,7 +34807,7 @@
         <v>1246</v>
       </c>
     </row>
-    <row r="202" spans="1:6" ht="70">
+    <row r="202" spans="1:6" ht="70" hidden="1">
       <c r="A202" s="18">
         <v>193</v>
       </c>
@@ -34826,7 +34827,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="203" spans="1:6" ht="56">
+    <row r="203" spans="1:6" ht="56" hidden="1">
       <c r="A203" s="18">
         <v>194</v>
       </c>
@@ -34846,7 +34847,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="204" spans="1:6" ht="42">
+    <row r="204" spans="1:6" ht="42" hidden="1">
       <c r="A204" s="18">
         <v>195</v>
       </c>
@@ -34866,7 +34867,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="205" spans="1:6" ht="14">
+    <row r="205" spans="1:6" ht="14" hidden="1">
       <c r="A205" s="18">
         <v>196</v>
       </c>
@@ -34886,7 +34887,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="206" spans="1:6" ht="14">
+    <row r="206" spans="1:6" ht="14" hidden="1">
       <c r="A206" s="18">
         <v>197</v>
       </c>
@@ -34906,7 +34907,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="207" spans="1:6" ht="14">
+    <row r="207" spans="1:6" ht="14" hidden="1">
       <c r="A207" s="18">
         <v>198</v>
       </c>
@@ -34926,7 +34927,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="208" spans="1:6" ht="14">
+    <row r="208" spans="1:6" ht="14" hidden="1">
       <c r="A208" s="18">
         <v>199</v>
       </c>
@@ -34946,7 +34947,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="209" spans="1:6" ht="28">
+    <row r="209" spans="1:6" ht="28" hidden="1">
       <c r="A209" s="18">
         <v>200</v>
       </c>
@@ -34966,7 +34967,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="210" spans="1:6" ht="14">
+    <row r="210" spans="1:6" ht="14" hidden="1">
       <c r="A210" s="18">
         <v>201</v>
       </c>
@@ -34986,7 +34987,7 @@
         <v>1274</v>
       </c>
     </row>
-    <row r="211" spans="1:6" ht="42">
+    <row r="211" spans="1:6" ht="42" hidden="1">
       <c r="A211" s="18">
         <v>202</v>
       </c>
@@ -35006,7 +35007,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="212" spans="1:6" ht="14">
+    <row r="212" spans="1:6" ht="14" hidden="1">
       <c r="A212" s="18">
         <v>203</v>
       </c>
@@ -35026,7 +35027,7 @@
         <v>1070</v>
       </c>
     </row>
-    <row r="213" spans="1:6" ht="28">
+    <row r="213" spans="1:6" ht="28" hidden="1">
       <c r="A213" s="18">
         <v>204</v>
       </c>
@@ -35046,7 +35047,7 @@
         <v>1284</v>
       </c>
     </row>
-    <row r="214" spans="1:6" ht="14">
+    <row r="214" spans="1:6" ht="14" hidden="1">
       <c r="A214" s="18">
         <v>205</v>
       </c>
@@ -35066,7 +35067,7 @@
         <v>1287</v>
       </c>
     </row>
-    <row r="215" spans="1:6" ht="14">
+    <row r="215" spans="1:6" ht="14" hidden="1">
       <c r="A215" s="18">
         <v>206</v>
       </c>
@@ -35086,7 +35087,7 @@
         <v>1290</v>
       </c>
     </row>
-    <row r="216" spans="1:6" ht="14">
+    <row r="216" spans="1:6" ht="14" hidden="1">
       <c r="A216" s="18">
         <v>207</v>
       </c>
@@ -35106,7 +35107,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="217" spans="1:6" ht="14">
+    <row r="217" spans="1:6" ht="14" hidden="1">
       <c r="A217" s="18">
         <v>208</v>
       </c>
@@ -35126,7 +35127,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="218" spans="1:6" ht="14">
+    <row r="218" spans="1:6" ht="14" hidden="1">
       <c r="A218" s="18">
         <v>209</v>
       </c>
@@ -35146,7 +35147,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="219" spans="1:6" ht="14">
+    <row r="219" spans="1:6" ht="14" hidden="1">
       <c r="A219" s="18">
         <v>210</v>
       </c>
@@ -35166,7 +35167,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="220" spans="1:6" ht="42">
+    <row r="220" spans="1:6" ht="42" hidden="1">
       <c r="A220" s="18">
         <v>211</v>
       </c>
@@ -35186,7 +35187,7 @@
         <v>1302</v>
       </c>
     </row>
-    <row r="221" spans="1:6" ht="42">
+    <row r="221" spans="1:6" ht="42" hidden="1">
       <c r="A221" s="18">
         <v>212</v>
       </c>
@@ -35206,7 +35207,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="222" spans="1:6" ht="28">
+    <row r="222" spans="1:6" ht="28" hidden="1">
       <c r="A222" s="18">
         <v>213</v>
       </c>
@@ -35226,7 +35227,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="223" spans="1:6" ht="12.75" customHeight="1">
+    <row r="223" spans="1:6" ht="12.75" hidden="1" customHeight="1">
       <c r="A223" s="18">
         <v>214</v>
       </c>
@@ -35246,7 +35247,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="224" spans="1:6" ht="12.75" customHeight="1">
+    <row r="224" spans="1:6" ht="12.75" hidden="1" customHeight="1">
       <c r="A224" s="18">
         <v>215</v>
       </c>
@@ -35266,7 +35267,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="225" spans="1:239" ht="12.75" customHeight="1">
+    <row r="225" spans="1:239" ht="12.75" hidden="1" customHeight="1">
       <c r="A225" s="18">
         <v>216</v>
       </c>
@@ -35286,7 +35287,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="226" spans="1:239" ht="12.75" customHeight="1">
+    <row r="226" spans="1:239" ht="12.75" hidden="1" customHeight="1">
       <c r="A226" s="18">
         <v>217</v>
       </c>
@@ -35306,7 +35307,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="227" spans="1:239" ht="32.25" customHeight="1">
+    <row r="227" spans="1:239" ht="32.25" hidden="1" customHeight="1">
       <c r="A227" s="18">
         <v>218</v>
       </c>
@@ -35326,7 +35327,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="228" spans="1:239" ht="42">
+    <row r="228" spans="1:239" ht="42" hidden="1">
       <c r="A228" s="18">
         <v>219</v>
       </c>
@@ -35346,7 +35347,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="229" spans="1:239" ht="28">
+    <row r="229" spans="1:239" ht="28" hidden="1">
       <c r="A229" s="18">
         <v>220</v>
       </c>
@@ -35366,7 +35367,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="230" spans="1:239" ht="28">
+    <row r="230" spans="1:239" ht="28" hidden="1">
       <c r="A230" s="18">
         <v>221</v>
       </c>
@@ -35386,7 +35387,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="231" spans="1:239" ht="28">
+    <row r="231" spans="1:239" ht="28" hidden="1">
       <c r="A231" s="18">
         <v>222</v>
       </c>
@@ -35406,7 +35407,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="232" spans="1:239" ht="14">
+    <row r="232" spans="1:239" ht="14" hidden="1">
       <c r="A232" s="18">
         <v>223</v>
       </c>
@@ -35426,7 +35427,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="233" spans="1:239" ht="14">
+    <row r="233" spans="1:239" ht="14" hidden="1">
       <c r="A233" s="18">
         <v>224</v>
       </c>
@@ -35446,7 +35447,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="234" spans="1:239" ht="14">
+    <row r="234" spans="1:239" ht="14" hidden="1">
       <c r="A234" s="18">
         <v>225</v>
       </c>
@@ -35466,7 +35467,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="235" spans="1:239" ht="28">
+    <row r="235" spans="1:239" ht="28" hidden="1">
       <c r="A235" s="18">
         <v>226</v>
       </c>
@@ -35486,7 +35487,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="236" spans="1:239" ht="14">
+    <row r="236" spans="1:239" ht="14" hidden="1">
       <c r="A236" s="18">
         <v>227</v>
       </c>
@@ -35506,7 +35507,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="237" spans="1:239" ht="56">
+    <row r="237" spans="1:239" ht="56" hidden="1">
       <c r="A237" s="18">
         <v>228</v>
       </c>
@@ -35527,7 +35528,7 @@
       </c>
       <c r="IE237" s="22"/>
     </row>
-    <row r="238" spans="1:239" ht="56">
+    <row r="238" spans="1:239" ht="56" hidden="1">
       <c r="A238" s="18">
         <v>229</v>
       </c>
@@ -35548,7 +35549,7 @@
       </c>
       <c r="IE238" s="22"/>
     </row>
-    <row r="239" spans="1:239" ht="42">
+    <row r="239" spans="1:239" ht="42" hidden="1">
       <c r="A239" s="18">
         <v>230</v>
       </c>
@@ -35568,7 +35569,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="240" spans="1:239" ht="42">
+    <row r="240" spans="1:239" ht="42" hidden="1">
       <c r="A240" s="18">
         <v>231</v>
       </c>
@@ -35588,7 +35589,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="241" spans="1:239" ht="42">
+    <row r="241" spans="1:239" ht="42" hidden="1">
       <c r="A241" s="18">
         <v>232</v>
       </c>
@@ -35608,7 +35609,7 @@
         <v>1367</v>
       </c>
     </row>
-    <row r="242" spans="1:239" ht="42">
+    <row r="242" spans="1:239" ht="42" hidden="1">
       <c r="A242" s="18">
         <v>233</v>
       </c>
@@ -35628,7 +35629,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="243" spans="1:239" ht="14">
+    <row r="243" spans="1:239" ht="14" hidden="1">
       <c r="A243" s="18">
         <v>234</v>
       </c>
@@ -35648,7 +35649,7 @@
         <v>1371</v>
       </c>
     </row>
-    <row r="244" spans="1:239" ht="14">
+    <row r="244" spans="1:239" ht="14" hidden="1">
       <c r="A244" s="18">
         <v>235</v>
       </c>
@@ -35668,7 +35669,7 @@
         <v>1371</v>
       </c>
     </row>
-    <row r="245" spans="1:239" ht="14">
+    <row r="245" spans="1:239" ht="14" hidden="1">
       <c r="A245" s="18">
         <v>236</v>
       </c>
@@ -35688,7 +35689,7 @@
         <v>1371</v>
       </c>
     </row>
-    <row r="246" spans="1:239" ht="14">
+    <row r="246" spans="1:239" ht="14" hidden="1">
       <c r="A246" s="18">
         <v>237</v>
       </c>
@@ -35708,7 +35709,7 @@
         <v>1070</v>
       </c>
     </row>
-    <row r="247" spans="1:239" ht="14">
+    <row r="247" spans="1:239" ht="14" hidden="1">
       <c r="A247" s="18">
         <v>238</v>
       </c>
@@ -35728,7 +35729,7 @@
         <v>1070</v>
       </c>
     </row>
-    <row r="248" spans="1:239" ht="28">
+    <row r="248" spans="1:239" ht="28" hidden="1">
       <c r="A248" s="18">
         <v>239</v>
       </c>
@@ -35981,7 +35982,7 @@
       <c r="ID248" s="19"/>
       <c r="IE248" s="19"/>
     </row>
-    <row r="249" spans="1:239" ht="70">
+    <row r="249" spans="1:239" ht="70" hidden="1">
       <c r="A249" s="18">
         <v>240</v>
       </c>
@@ -36234,7 +36235,7 @@
       <c r="ID249" s="19"/>
       <c r="IE249" s="19"/>
     </row>
-    <row r="250" spans="1:239" ht="28">
+    <row r="250" spans="1:239" ht="28" hidden="1">
       <c r="A250" s="18">
         <v>241</v>
       </c>
@@ -36487,7 +36488,7 @@
       <c r="ID250" s="19"/>
       <c r="IE250" s="19"/>
     </row>
-    <row r="251" spans="1:239" ht="14">
+    <row r="251" spans="1:239" ht="14" hidden="1">
       <c r="A251" s="18">
         <v>242</v>
       </c>
@@ -36738,7 +36739,7 @@
       <c r="ID251" s="19"/>
       <c r="IE251" s="19"/>
     </row>
-    <row r="252" spans="1:239" ht="28">
+    <row r="252" spans="1:239" ht="28" hidden="1">
       <c r="A252" s="18">
         <v>243</v>
       </c>
@@ -36991,7 +36992,7 @@
       <c r="ID252" s="19"/>
       <c r="IE252" s="19"/>
     </row>
-    <row r="253" spans="1:239" ht="14">
+    <row r="253" spans="1:239" ht="14" hidden="1">
       <c r="A253" s="18">
         <v>244</v>
       </c>
@@ -37244,7 +37245,7 @@
       <c r="ID253" s="19"/>
       <c r="IE253" s="19"/>
     </row>
-    <row r="254" spans="1:239" ht="14">
+    <row r="254" spans="1:239" ht="14" hidden="1">
       <c r="A254" s="18">
         <v>245</v>
       </c>
@@ -37497,7 +37498,7 @@
       <c r="ID254" s="19"/>
       <c r="IE254" s="19"/>
     </row>
-    <row r="255" spans="1:239" ht="56">
+    <row r="255" spans="1:239" ht="56" hidden="1">
       <c r="A255" s="18">
         <v>246</v>
       </c>
@@ -37517,7 +37518,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="256" spans="1:239" s="33" customFormat="1" ht="45.5" customHeight="1">
+    <row r="256" spans="1:239" s="33" customFormat="1" ht="45.5" hidden="1" customHeight="1">
       <c r="A256" s="331" t="s">
         <v>1393</v>
       </c>
@@ -37760,7 +37761,7 @@
       <c r="ID256"/>
       <c r="IE256"/>
     </row>
-    <row r="257" spans="1:239" s="36" customFormat="1" ht="24" customHeight="1">
+    <row r="257" spans="1:239" s="36" customFormat="1" ht="24" hidden="1" customHeight="1">
       <c r="A257" s="35" t="s">
         <v>54</v>
       </c>
@@ -38013,7 +38014,7 @@
       <c r="ID257"/>
       <c r="IE257"/>
     </row>
-    <row r="258" spans="1:239" ht="14">
+    <row r="258" spans="1:239" ht="14" hidden="1">
       <c r="A258" s="18">
         <v>247</v>
       </c>
@@ -38033,7 +38034,7 @@
         <v>1398</v>
       </c>
     </row>
-    <row r="259" spans="1:239" ht="14">
+    <row r="259" spans="1:239" ht="14" hidden="1">
       <c r="A259" s="18">
         <v>248</v>
       </c>
@@ -38054,7 +38055,7 @@
         <v>1398</v>
       </c>
     </row>
-    <row r="260" spans="1:239" ht="14">
+    <row r="260" spans="1:239" ht="14" hidden="1">
       <c r="A260" s="18">
         <v>249</v>
       </c>
@@ -38075,7 +38076,7 @@
         <v>1398</v>
       </c>
     </row>
-    <row r="261" spans="1:239" s="37" customFormat="1" ht="14">
+    <row r="261" spans="1:239" s="37" customFormat="1" ht="14" hidden="1">
       <c r="A261" s="18">
         <v>250</v>
       </c>
@@ -38350,7 +38351,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="263" spans="1:239" ht="14">
+    <row r="263" spans="1:239" ht="14" hidden="1">
       <c r="A263" s="18">
         <v>252</v>
       </c>
@@ -38371,7 +38372,7 @@
         <v>1411</v>
       </c>
     </row>
-    <row r="264" spans="1:239" ht="14">
+    <row r="264" spans="1:239" ht="14" hidden="1">
       <c r="A264" s="18">
         <v>253</v>
       </c>
@@ -38392,7 +38393,7 @@
         <v>1414</v>
       </c>
     </row>
-    <row r="265" spans="1:239" ht="14">
+    <row r="265" spans="1:239" ht="14" hidden="1">
       <c r="A265" s="18">
         <v>254</v>
       </c>
@@ -38413,7 +38414,7 @@
         <v>1398</v>
       </c>
     </row>
-    <row r="266" spans="1:239" ht="14">
+    <row r="266" spans="1:239" ht="14" hidden="1">
       <c r="A266" s="18">
         <v>255</v>
       </c>
@@ -38434,7 +38435,7 @@
         <v>1398</v>
       </c>
     </row>
-    <row r="267" spans="1:239" ht="14">
+    <row r="267" spans="1:239" ht="14" hidden="1">
       <c r="A267" s="18">
         <v>256</v>
       </c>
@@ -38455,7 +38456,7 @@
         <v>1398</v>
       </c>
     </row>
-    <row r="268" spans="1:239" ht="14">
+    <row r="268" spans="1:239" ht="14" hidden="1">
       <c r="A268" s="18">
         <v>257</v>
       </c>
@@ -38476,7 +38477,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="269" spans="1:239" ht="14">
+    <row r="269" spans="1:239" ht="14" hidden="1">
       <c r="A269" s="18">
         <v>258</v>
       </c>
@@ -38497,7 +38498,7 @@
         <v>1398</v>
       </c>
     </row>
-    <row r="270" spans="1:239" ht="14">
+    <row r="270" spans="1:239" ht="14" hidden="1">
       <c r="A270" s="18">
         <v>259</v>
       </c>
@@ -38518,7 +38519,7 @@
         <v>1398</v>
       </c>
     </row>
-    <row r="271" spans="1:239" ht="14">
+    <row r="271" spans="1:239" ht="14" hidden="1">
       <c r="A271" s="18">
         <v>260</v>
       </c>
@@ -38539,7 +38540,7 @@
         <v>1398</v>
       </c>
     </row>
-    <row r="272" spans="1:239" ht="14">
+    <row r="272" spans="1:239" ht="14" hidden="1">
       <c r="A272" s="18">
         <v>261</v>
       </c>
@@ -38560,7 +38561,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="273" spans="1:6" ht="14">
+    <row r="273" spans="1:6" ht="14" hidden="1">
       <c r="A273" s="249">
         <v>262</v>
       </c>
@@ -38581,7 +38582,7 @@
         <v>1430</v>
       </c>
     </row>
-    <row r="274" spans="1:6" ht="14">
+    <row r="274" spans="1:6" ht="14" hidden="1">
       <c r="A274" s="249">
         <v>263</v>
       </c>
@@ -38600,7 +38601,7 @@
       </c>
       <c r="F274" s="326"/>
     </row>
-    <row r="275" spans="1:6" ht="14">
+    <row r="275" spans="1:6" ht="14" hidden="1">
       <c r="A275" s="249">
         <v>264</v>
       </c>
@@ -38619,7 +38620,7 @@
       </c>
       <c r="F275" s="326"/>
     </row>
-    <row r="276" spans="1:6" ht="14">
+    <row r="276" spans="1:6" ht="14" hidden="1">
       <c r="A276" s="249">
         <v>265</v>
       </c>
@@ -38638,7 +38639,7 @@
       </c>
       <c r="F276" s="326"/>
     </row>
-    <row r="277" spans="1:6" ht="14">
+    <row r="277" spans="1:6" ht="14" hidden="1">
       <c r="A277" s="249">
         <v>266</v>
       </c>
@@ -38657,7 +38658,7 @@
       </c>
       <c r="F277" s="326"/>
     </row>
-    <row r="278" spans="1:6" ht="14">
+    <row r="278" spans="1:6" ht="14" hidden="1">
       <c r="A278" s="249">
         <v>267</v>
       </c>
@@ -38676,7 +38677,7 @@
       </c>
       <c r="F278" s="326"/>
     </row>
-    <row r="279" spans="1:6" ht="56">
+    <row r="279" spans="1:6" ht="56" hidden="1">
       <c r="A279" s="255">
         <v>268</v>
       </c>
@@ -38697,7 +38698,7 @@
         <v>1443</v>
       </c>
     </row>
-    <row r="280" spans="1:6" ht="28">
+    <row r="280" spans="1:6" ht="28" hidden="1">
       <c r="A280" s="249">
         <v>269</v>
       </c>
@@ -38739,7 +38740,7 @@
         <v>1448</v>
       </c>
     </row>
-    <row r="282" spans="1:6" ht="14">
+    <row r="282" spans="1:6" ht="14" hidden="1">
       <c r="A282" s="249">
         <v>271</v>
       </c>
@@ -38760,7 +38761,7 @@
         <v>1411</v>
       </c>
     </row>
-    <row r="283" spans="1:6" ht="28">
+    <row r="283" spans="1:6" ht="28" hidden="1">
       <c r="A283" s="249">
         <v>272</v>
       </c>
@@ -38781,7 +38782,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="284" spans="1:6" ht="14">
+    <row r="284" spans="1:6" ht="14" hidden="1">
       <c r="A284" s="249">
         <v>273</v>
       </c>
@@ -38802,7 +38803,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="285" spans="1:6" ht="14">
+    <row r="285" spans="1:6" ht="14" hidden="1">
       <c r="A285" s="18">
         <v>274</v>
       </c>
@@ -38823,7 +38824,7 @@
         <v>1398</v>
       </c>
     </row>
-    <row r="286" spans="1:6" ht="14">
+    <row r="286" spans="1:6" ht="14" hidden="1">
       <c r="A286" s="18">
         <v>275</v>
       </c>
@@ -38844,7 +38845,7 @@
         <v>1398</v>
       </c>
     </row>
-    <row r="287" spans="1:6" ht="14">
+    <row r="287" spans="1:6" ht="14" hidden="1">
       <c r="A287" s="18">
         <v>276</v>
       </c>
@@ -38865,7 +38866,7 @@
         <v>1398</v>
       </c>
     </row>
-    <row r="288" spans="1:6" ht="14">
+    <row r="288" spans="1:6" ht="14" hidden="1">
       <c r="A288" s="18">
         <v>277</v>
       </c>
@@ -38886,7 +38887,7 @@
         <v>1459</v>
       </c>
     </row>
-    <row r="289" spans="1:239" ht="14">
+    <row r="289" spans="1:239" ht="14" hidden="1">
       <c r="A289" s="18">
         <v>278</v>
       </c>
@@ -38907,7 +38908,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="290" spans="1:239" ht="14">
+    <row r="290" spans="1:239" ht="14" hidden="1">
       <c r="A290" s="18">
         <v>279</v>
       </c>
@@ -38928,7 +38929,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="291" spans="1:239" s="16" customFormat="1" ht="14">
+    <row r="291" spans="1:239" s="16" customFormat="1" ht="14" hidden="1">
       <c r="A291" s="18">
         <v>280</v>
       </c>
@@ -39181,7 +39182,7 @@
       <c r="ID291" s="19"/>
       <c r="IE291" s="19"/>
     </row>
-    <row r="292" spans="1:239" s="16" customFormat="1" ht="14">
+    <row r="292" spans="1:239" s="16" customFormat="1" ht="14" hidden="1">
       <c r="A292" s="18">
         <v>281</v>
       </c>
@@ -39434,7 +39435,7 @@
       <c r="ID292" s="19"/>
       <c r="IE292" s="19"/>
     </row>
-    <row r="293" spans="1:239" ht="14">
+    <row r="293" spans="1:239" ht="14" hidden="1">
       <c r="A293" s="18">
         <v>282</v>
       </c>
@@ -39454,7 +39455,7 @@
         <v>1471</v>
       </c>
     </row>
-    <row r="294" spans="1:239" ht="42">
+    <row r="294" spans="1:239" ht="42" hidden="1">
       <c r="A294" s="18">
         <v>283</v>
       </c>
@@ -39475,7 +39476,7 @@
         <v>1474</v>
       </c>
     </row>
-    <row r="295" spans="1:239" ht="14">
+    <row r="295" spans="1:239" ht="14" hidden="1">
       <c r="A295" s="18">
         <v>284</v>
       </c>
@@ -39496,7 +39497,7 @@
         <v>1477</v>
       </c>
     </row>
-    <row r="296" spans="1:239" ht="42">
+    <row r="296" spans="1:239" ht="42" hidden="1">
       <c r="A296" s="18">
         <v>285</v>
       </c>
@@ -39517,7 +39518,7 @@
         <v>1474</v>
       </c>
     </row>
-    <row r="297" spans="1:239" ht="14">
+    <row r="297" spans="1:239" ht="14" hidden="1">
       <c r="A297" s="18">
         <v>286</v>
       </c>
@@ -39538,7 +39539,7 @@
         <v>1482</v>
       </c>
     </row>
-    <row r="298" spans="1:239" ht="42">
+    <row r="298" spans="1:239" ht="42" hidden="1">
       <c r="A298" s="18">
         <v>287</v>
       </c>
@@ -39559,7 +39560,7 @@
         <v>1474</v>
       </c>
     </row>
-    <row r="299" spans="1:239" ht="14">
+    <row r="299" spans="1:239" ht="14" hidden="1">
       <c r="A299" s="18">
         <v>288</v>
       </c>
@@ -39580,7 +39581,7 @@
         <v>1487</v>
       </c>
     </row>
-    <row r="300" spans="1:239" ht="42">
+    <row r="300" spans="1:239" ht="42" hidden="1">
       <c r="A300" s="18">
         <v>289</v>
       </c>
@@ -39601,7 +39602,7 @@
         <v>1474</v>
       </c>
     </row>
-    <row r="301" spans="1:239" s="38" customFormat="1" ht="345">
+    <row r="301" spans="1:239" s="38" customFormat="1" ht="345" hidden="1">
       <c r="A301" s="18">
         <v>290</v>
       </c>
@@ -39854,7 +39855,7 @@
       <c r="ID301"/>
       <c r="IE301"/>
     </row>
-    <row r="302" spans="1:239" s="38" customFormat="1" ht="14">
+    <row r="302" spans="1:239" s="38" customFormat="1" ht="14" hidden="1">
       <c r="A302" s="18">
         <v>291</v>
       </c>
@@ -40107,7 +40108,7 @@
       <c r="ID302"/>
       <c r="IE302"/>
     </row>
-    <row r="303" spans="1:239" ht="12.75" customHeight="1">
+    <row r="303" spans="1:239" ht="12.75" hidden="1" customHeight="1">
       <c r="A303" s="18">
         <v>292</v>
       </c>
@@ -40127,7 +40128,7 @@
         <v>1498</v>
       </c>
     </row>
-    <row r="304" spans="1:239" ht="52.5" customHeight="1">
+    <row r="304" spans="1:239" ht="52.5" hidden="1" customHeight="1">
       <c r="A304" s="18">
         <v>293</v>
       </c>
@@ -40148,7 +40149,7 @@
         <v>1501</v>
       </c>
     </row>
-    <row r="305" spans="1:239" ht="266">
+    <row r="305" spans="1:239" ht="266" hidden="1">
       <c r="A305" s="18">
         <v>294</v>
       </c>
@@ -40169,7 +40170,7 @@
         <v>1504</v>
       </c>
     </row>
-    <row r="306" spans="1:239" ht="14">
+    <row r="306" spans="1:239" ht="14" hidden="1">
       <c r="A306" s="18">
         <v>295</v>
       </c>
@@ -40190,7 +40191,7 @@
         <v>1498</v>
       </c>
     </row>
-    <row r="307" spans="1:239" ht="14">
+    <row r="307" spans="1:239" ht="14" hidden="1">
       <c r="A307" s="18">
         <v>296</v>
       </c>
@@ -40211,7 +40212,7 @@
         <v>1498</v>
       </c>
     </row>
-    <row r="308" spans="1:239" ht="266">
+    <row r="308" spans="1:239" ht="266" hidden="1">
       <c r="A308" s="18">
         <v>297</v>
       </c>
@@ -40232,7 +40233,7 @@
         <v>1504</v>
       </c>
     </row>
-    <row r="309" spans="1:239" ht="14">
+    <row r="309" spans="1:239" ht="14" hidden="1">
       <c r="A309" s="18">
         <v>298</v>
       </c>
@@ -40253,7 +40254,7 @@
         <v>1513</v>
       </c>
     </row>
-    <row r="310" spans="1:239" ht="14">
+    <row r="310" spans="1:239" ht="14" hidden="1">
       <c r="A310" s="18">
         <v>299</v>
       </c>
@@ -40274,7 +40275,7 @@
         <v>1513</v>
       </c>
     </row>
-    <row r="311" spans="1:239" ht="14">
+    <row r="311" spans="1:239" ht="14" hidden="1">
       <c r="A311" s="18">
         <v>300</v>
       </c>
@@ -40295,7 +40296,7 @@
         <v>1513</v>
       </c>
     </row>
-    <row r="312" spans="1:239" ht="14">
+    <row r="312" spans="1:239" ht="14" hidden="1">
       <c r="A312" s="18">
         <v>301</v>
       </c>
@@ -40316,7 +40317,7 @@
         <v>1513</v>
       </c>
     </row>
-    <row r="313" spans="1:239" ht="14">
+    <row r="313" spans="1:239" ht="14" hidden="1">
       <c r="A313" s="18">
         <v>302</v>
       </c>
@@ -40337,7 +40338,7 @@
         <v>1522</v>
       </c>
     </row>
-    <row r="314" spans="1:239" ht="14">
+    <row r="314" spans="1:239" ht="14" hidden="1">
       <c r="A314" s="18">
         <v>303</v>
       </c>
@@ -40358,7 +40359,7 @@
         <v>1522</v>
       </c>
     </row>
-    <row r="315" spans="1:239" s="38" customFormat="1" ht="14">
+    <row r="315" spans="1:239" s="38" customFormat="1" ht="14" hidden="1">
       <c r="A315" s="18">
         <v>304</v>
       </c>
@@ -40612,7 +40613,7 @@
       <c r="ID315"/>
       <c r="IE315"/>
     </row>
-    <row r="316" spans="1:239" s="33" customFormat="1" ht="30.75" customHeight="1">
+    <row r="316" spans="1:239" s="33" customFormat="1" ht="30.75" hidden="1" customHeight="1">
       <c r="A316" s="331" t="s">
         <v>1528</v>
       </c>
@@ -40855,7 +40856,7 @@
       <c r="ID316"/>
       <c r="IE316"/>
     </row>
-    <row r="317" spans="1:239" s="36" customFormat="1" ht="24" customHeight="1">
+    <row r="317" spans="1:239" s="36" customFormat="1" ht="24" hidden="1" customHeight="1">
       <c r="A317" s="35" t="s">
         <v>54</v>
       </c>
@@ -41108,7 +41109,7 @@
       <c r="ID317"/>
       <c r="IE317"/>
     </row>
-    <row r="318" spans="1:239" ht="28">
+    <row r="318" spans="1:239" ht="28" hidden="1">
       <c r="A318" s="18">
         <v>305</v>
       </c>
@@ -41129,7 +41130,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="319" spans="1:239" ht="14">
+    <row r="319" spans="1:239" ht="14" hidden="1">
       <c r="A319" s="18">
         <v>306</v>
       </c>
@@ -41150,7 +41151,7 @@
         <v>1533</v>
       </c>
     </row>
-    <row r="320" spans="1:239" ht="28">
+    <row r="320" spans="1:239" ht="28" hidden="1">
       <c r="A320" s="18">
         <v>307</v>
       </c>
@@ -41171,7 +41172,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="321" spans="1:6" ht="14">
+    <row r="321" spans="1:6" ht="14" hidden="1">
       <c r="A321" s="18">
         <v>308</v>
       </c>
@@ -41192,7 +41193,7 @@
         <v>1533</v>
       </c>
     </row>
-    <row r="322" spans="1:6" ht="14">
+    <row r="322" spans="1:6" ht="14" hidden="1">
       <c r="A322" s="18">
         <v>309</v>
       </c>
@@ -41213,7 +41214,7 @@
         <v>1540</v>
       </c>
     </row>
-    <row r="323" spans="1:6" ht="14">
+    <row r="323" spans="1:6" ht="14" hidden="1">
       <c r="A323" s="18">
         <v>310</v>
       </c>
@@ -41232,7 +41233,7 @@
       </c>
       <c r="F323" s="325"/>
     </row>
-    <row r="324" spans="1:6" ht="14">
+    <row r="324" spans="1:6" ht="14" hidden="1">
       <c r="A324" s="18">
         <v>311</v>
       </c>
@@ -41251,7 +41252,7 @@
       </c>
       <c r="F324" s="325"/>
     </row>
-    <row r="325" spans="1:6" ht="14">
+    <row r="325" spans="1:6" ht="14" hidden="1">
       <c r="A325" s="18">
         <v>312</v>
       </c>
@@ -41270,7 +41271,7 @@
       </c>
       <c r="F325" s="325"/>
     </row>
-    <row r="326" spans="1:6" ht="14">
+    <row r="326" spans="1:6" ht="14" hidden="1">
       <c r="A326" s="18">
         <v>313</v>
       </c>
@@ -41289,7 +41290,7 @@
       </c>
       <c r="F326" s="325"/>
     </row>
-    <row r="327" spans="1:6" ht="14">
+    <row r="327" spans="1:6" ht="14" hidden="1">
       <c r="A327" s="18">
         <v>314</v>
       </c>
@@ -41308,7 +41309,7 @@
       </c>
       <c r="F327" s="325"/>
     </row>
-    <row r="328" spans="1:6" ht="56">
+    <row r="328" spans="1:6" ht="56" hidden="1">
       <c r="A328" s="18">
         <v>315</v>
       </c>
@@ -41329,7 +41330,7 @@
         <v>1553</v>
       </c>
     </row>
-    <row r="329" spans="1:6" ht="28">
+    <row r="329" spans="1:6" ht="28" hidden="1">
       <c r="A329" s="18">
         <v>316</v>
       </c>
@@ -41371,7 +41372,7 @@
         <v>1448</v>
       </c>
     </row>
-    <row r="331" spans="1:6" ht="14">
+    <row r="331" spans="1:6" ht="14" hidden="1">
       <c r="A331" s="18">
         <v>318</v>
       </c>
@@ -41392,7 +41393,7 @@
         <v>1411</v>
       </c>
     </row>
-    <row r="332" spans="1:6" ht="14">
+    <row r="332" spans="1:6" ht="14" hidden="1">
       <c r="A332" s="18">
         <v>319</v>
       </c>
@@ -41413,7 +41414,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="333" spans="1:6" ht="14">
+    <row r="333" spans="1:6" ht="14" hidden="1">
       <c r="A333" s="18">
         <v>320</v>
       </c>
@@ -41434,7 +41435,7 @@
         <v>1564</v>
       </c>
     </row>
-    <row r="334" spans="1:6" ht="28">
+    <row r="334" spans="1:6" ht="28" hidden="1">
       <c r="A334" s="18">
         <v>321</v>
       </c>
@@ -41455,7 +41456,7 @@
         <v>1567</v>
       </c>
     </row>
-    <row r="335" spans="1:6" ht="14">
+    <row r="335" spans="1:6" ht="14" hidden="1">
       <c r="A335" s="18">
         <v>322</v>
       </c>
@@ -41476,7 +41477,7 @@
         <v>1570</v>
       </c>
     </row>
-    <row r="336" spans="1:6" ht="42">
+    <row r="336" spans="1:6" ht="42" hidden="1">
       <c r="A336" s="18">
         <v>323</v>
       </c>
@@ -41497,7 +41498,7 @@
         <v>1573</v>
       </c>
     </row>
-    <row r="337" spans="1:239" ht="42">
+    <row r="337" spans="1:239" ht="42" hidden="1">
       <c r="A337" s="18">
         <v>324</v>
       </c>
@@ -41518,7 +41519,7 @@
         <v>1573</v>
       </c>
     </row>
-    <row r="338" spans="1:239" ht="28">
+    <row r="338" spans="1:239" ht="28" hidden="1">
       <c r="A338" s="18">
         <v>325</v>
       </c>
@@ -41539,7 +41540,7 @@
         <v>1578</v>
       </c>
     </row>
-    <row r="339" spans="1:239" ht="14">
+    <row r="339" spans="1:239" ht="14" hidden="1">
       <c r="A339" s="18">
         <v>326</v>
       </c>
@@ -41560,7 +41561,7 @@
         <v>1398</v>
       </c>
     </row>
-    <row r="340" spans="1:239" ht="14">
+    <row r="340" spans="1:239" ht="14" hidden="1">
       <c r="A340" s="18">
         <v>327</v>
       </c>
@@ -41581,7 +41582,7 @@
         <v>1583</v>
       </c>
     </row>
-    <row r="341" spans="1:239" ht="14">
+    <row r="341" spans="1:239" ht="14" hidden="1">
       <c r="A341" s="18">
         <v>328</v>
       </c>
@@ -41602,7 +41603,7 @@
         <v>1398</v>
       </c>
     </row>
-    <row r="342" spans="1:239" ht="14">
+    <row r="342" spans="1:239" ht="14" hidden="1">
       <c r="A342" s="18">
         <v>329</v>
       </c>
@@ -41623,7 +41624,7 @@
         <v>1588</v>
       </c>
     </row>
-    <row r="343" spans="1:239" ht="98">
+    <row r="343" spans="1:239" ht="98" hidden="1">
       <c r="A343" s="18">
         <v>330</v>
       </c>
@@ -41644,7 +41645,7 @@
         <v>1591</v>
       </c>
     </row>
-    <row r="344" spans="1:239" s="38" customFormat="1" ht="14">
+    <row r="344" spans="1:239" s="38" customFormat="1" ht="14" hidden="1">
       <c r="A344" s="18">
         <v>331</v>
       </c>
@@ -41898,7 +41899,7 @@
       <c r="ID344"/>
       <c r="IE344"/>
     </row>
-    <row r="345" spans="1:239" ht="14">
+    <row r="345" spans="1:239" ht="14" hidden="1">
       <c r="A345" s="18">
         <v>332</v>
       </c>
@@ -41919,7 +41920,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="346" spans="1:239" ht="14">
+    <row r="346" spans="1:239" ht="14" hidden="1">
       <c r="A346" s="18">
         <v>333</v>
       </c>
@@ -41940,7 +41941,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="347" spans="1:239" ht="14">
+    <row r="347" spans="1:239" ht="14" hidden="1">
       <c r="A347" s="18">
         <v>334</v>
       </c>
@@ -41961,7 +41962,7 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="348" spans="1:239" ht="14">
+    <row r="348" spans="1:239" ht="14" hidden="1">
       <c r="A348" s="18">
         <v>335</v>
       </c>
@@ -41982,7 +41983,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="349" spans="1:239" ht="14">
+    <row r="349" spans="1:239" ht="14" hidden="1">
       <c r="A349" s="18">
         <v>336</v>
       </c>
@@ -42003,7 +42004,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="350" spans="1:239" ht="14">
+    <row r="350" spans="1:239" ht="14" hidden="1">
       <c r="A350" s="18">
         <v>337</v>
       </c>
@@ -42024,7 +42025,7 @@
         <v>1607</v>
       </c>
     </row>
-    <row r="351" spans="1:239" ht="14">
+    <row r="351" spans="1:239" ht="14" hidden="1">
       <c r="A351" s="18">
         <v>338</v>
       </c>
@@ -42045,7 +42046,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="352" spans="1:239" ht="14">
+    <row r="352" spans="1:239" ht="14" hidden="1">
       <c r="A352" s="18">
         <v>339</v>
       </c>
@@ -42066,7 +42067,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="353" spans="1:239" ht="28">
+    <row r="353" spans="1:239" ht="28" hidden="1">
       <c r="A353" s="18">
         <v>340</v>
       </c>
@@ -42087,7 +42088,7 @@
         <v>1613</v>
       </c>
     </row>
-    <row r="354" spans="1:239" ht="14">
+    <row r="354" spans="1:239" ht="14" hidden="1">
       <c r="A354" s="18">
         <v>341</v>
       </c>
@@ -42107,7 +42108,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="355" spans="1:239" ht="14">
+    <row r="355" spans="1:239" ht="14" hidden="1">
       <c r="A355" s="270">
         <v>342</v>
       </c>
@@ -42127,7 +42128,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="356" spans="1:239" ht="14">
+    <row r="356" spans="1:239" ht="14" hidden="1">
       <c r="A356" s="270">
         <v>343</v>
       </c>
@@ -42147,7 +42148,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="357" spans="1:239" ht="14">
+    <row r="357" spans="1:239" ht="14" hidden="1">
       <c r="A357" s="270">
         <v>344</v>
       </c>
@@ -42167,7 +42168,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="358" spans="1:239" ht="14">
+    <row r="358" spans="1:239" ht="14" hidden="1">
       <c r="A358" s="270">
         <v>345</v>
       </c>
@@ -42187,7 +42188,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="359" spans="1:239" ht="14">
+    <row r="359" spans="1:239" ht="14" hidden="1">
       <c r="A359" s="270">
         <v>346</v>
       </c>
@@ -42207,7 +42208,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="360" spans="1:239" ht="14">
+    <row r="360" spans="1:239" ht="14" hidden="1">
       <c r="A360" s="270">
         <v>347</v>
       </c>
@@ -42227,7 +42228,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="361" spans="1:239" ht="14">
+    <row r="361" spans="1:239" ht="14" hidden="1">
       <c r="A361" s="270">
         <v>348</v>
       </c>
@@ -42247,7 +42248,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="362" spans="1:239" ht="14">
+    <row r="362" spans="1:239" ht="14" hidden="1">
       <c r="A362" s="270">
         <v>349</v>
       </c>
@@ -42267,7 +42268,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="363" spans="1:239" ht="14">
+    <row r="363" spans="1:239" ht="14" hidden="1">
       <c r="A363" s="270">
         <v>350</v>
       </c>
@@ -42287,7 +42288,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="364" spans="1:239" ht="14">
+    <row r="364" spans="1:239" ht="14" hidden="1">
       <c r="A364" s="270">
         <v>351</v>
       </c>
@@ -42307,7 +42308,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="365" spans="1:239" ht="14">
+    <row r="365" spans="1:239" ht="14" hidden="1">
       <c r="A365" s="18">
         <v>352</v>
       </c>
@@ -42327,7 +42328,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="366" spans="1:239" s="39" customFormat="1" ht="14">
+    <row r="366" spans="1:239" s="39" customFormat="1" ht="14" hidden="1">
       <c r="A366" s="18">
         <v>353</v>
       </c>
@@ -42580,7 +42581,7 @@
       <c r="ID366" s="19"/>
       <c r="IE366" s="19"/>
     </row>
-    <row r="367" spans="1:239" s="39" customFormat="1">
+    <row r="367" spans="1:239" s="39" customFormat="1" hidden="1">
       <c r="B367" s="32">
         <f>SUM(B366+C366)-1</f>
         <v>4000</v>
@@ -42840,6 +42841,17 @@
       <c r="F369" s="41"/>
     </row>
   </sheetData>
+  <autoFilter ref="A8:IE367" xr:uid="{00000000-0001-0000-0300-000000000000}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="County of Birth"/>
+        <filter val="County of Birth (Literal)"/>
+        <filter val="Mother's Mailing Address County (Literal)"/>
+        <filter val="Mother's Residence County (Literal)"/>
+        <filter val="Residence of Mother--County"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <customSheetViews>
     <customSheetView guid="{F1069C25-F3CC-400B-8C16-E88E31027CCC}" fitToPage="1">
       <selection activeCell="A11" sqref="A11"/>
@@ -42877,8 +42889,8 @@
   </sheetPr>
   <dimension ref="A1:G376"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView topLeftCell="A146" zoomScale="209" zoomScaleNormal="209" workbookViewId="0">
+      <selection activeCell="D164" sqref="D164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13"/>
@@ -46981,7 +46993,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="209" spans="1:6" ht="28">
+    <row r="209" spans="1:6" ht="14">
       <c r="A209" s="132">
         <v>201</v>
       </c>
@@ -50447,7 +50459,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:G169"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
@@ -53923,7 +53935,7 @@
   </sheetPr>
   <dimension ref="A1:IE368"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView topLeftCell="A29" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
@@ -67977,10 +67989,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002752A2C1F044FE469AAF2142AB326B8C" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c07487fc32f7ac2d3b3707e982dea906">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c1a58edb-1ba6-4800-9942-1e1defaa36d6" xmlns:ns3="4b113022-9134-4b2e-abe8-26e86c9e296e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="be9eaf82d0c074f79785b0acc776d2a9" ns2:_="" ns3:_="">
     <xsd:import namespace="c1a58edb-1ba6-4800-9942-1e1defaa36d6"/>
@@ -68183,30 +68206,36 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6E1C13E-614F-4B48-A9FE-F6158F0F568F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4A36FDD-FA0C-40EF-989B-74F1F7876F18}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="4b113022-9134-4b2e-abe8-26e86c9e296e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="c1a58edb-1ba6-4800-9942-1e1defaa36d6"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2D8D0BD-9993-4EC8-86D1-0A7C5F6E1934}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D3F3134-699E-462F-8D9F-EA7A8DE51B1D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -68225,27 +68254,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2D8D0BD-9993-4EC8-86D1-0A7C5F6E1934}">
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6E1C13E-614F-4B48-A9FE-F6158F0F568F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4A36FDD-FA0C-40EF-989B-74F1F7876F18}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="4b113022-9134-4b2e-abe8-26e86c9e296e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="c1a58edb-1ba6-4800-9942-1e1defaa36d6"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fixed countyCode-->districtCode in data dictionary
</commit_message>
<xml_diff>
--- a/input/images/IJE_File_Layouts_Version_2021_FHIR.xlsx
+++ b/input/images/IJE_File_Layouts_Version_2021_FHIR.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skravitz/git/vrdr/input/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{000182D3-9D7C-C542-9CE1-848194F2FC20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68F5B87F-FC3D-DC4F-B884-DE4B69B40EF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4000" yWindow="500" windowWidth="63620" windowHeight="27760" tabRatio="779" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7734" uniqueCount="2690">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7734" uniqueCount="2693">
   <si>
     <t>u</t>
   </si>
@@ -9324,6 +9324,15 @@
   </si>
   <si>
     <t xml:space="preserve">extension[ SpouseAlive] </t>
+  </si>
+  <si>
+    <t>address.district.extension[districtCode]</t>
+  </si>
+  <si>
+    <t>address.district.extension[ districtCode].value</t>
+  </si>
+  <si>
+    <t>address.district.extension[ districtCode ]</t>
   </si>
 </sst>
 </file>
@@ -11879,8 +11888,8 @@
   </sheetPr>
   <dimension ref="A1:L284"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A154" zoomScale="220" zoomScaleNormal="220" zoomScaleSheetLayoutView="95" workbookViewId="0">
-      <selection activeCell="I164" sqref="I164"/>
+    <sheetView tabSelected="1" topLeftCell="G37" zoomScale="220" zoomScaleNormal="220" zoomScaleSheetLayoutView="95" workbookViewId="0">
+      <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13"/>
@@ -11914,7 +11923,7 @@
       </c>
       <c r="G1" s="296"/>
     </row>
-    <row r="2" spans="1:12" s="11" customFormat="1" ht="78">
+    <row r="2" spans="1:12" s="11" customFormat="1" ht="65">
       <c r="A2" s="228"/>
       <c r="B2" s="229"/>
       <c r="C2" s="229"/>
@@ -13181,7 +13190,7 @@
         <v>2318</v>
       </c>
       <c r="I38" s="16" t="s">
-        <v>2601</v>
+        <v>2692</v>
       </c>
       <c r="J38" s="16" t="s">
         <v>2320</v>
@@ -13447,7 +13456,7 @@
         <v>2347</v>
       </c>
       <c r="I45" s="16" t="s">
-        <v>2354</v>
+        <v>2690</v>
       </c>
       <c r="J45" s="16" t="s">
         <v>2320</v>
@@ -18838,7 +18847,7 @@
         <v>2449</v>
       </c>
       <c r="I198" s="16" t="s">
-        <v>2457</v>
+        <v>2691</v>
       </c>
       <c r="J198" s="16" t="s">
         <v>2320</v>
@@ -19746,7 +19755,7 @@
         <v>2325</v>
       </c>
     </row>
-    <row r="224" spans="1:12" ht="28">
+    <row r="224" spans="1:12" ht="14">
       <c r="A224" s="15">
         <f t="shared" si="10"/>
         <v>203</v>
@@ -32050,7 +32059,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="28" hidden="1">
+    <row r="64" spans="1:6" ht="14" hidden="1">
       <c r="A64" s="18">
         <v>55</v>
       </c>
@@ -67992,21 +68001,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002752A2C1F044FE469AAF2142AB326B8C" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c07487fc32f7ac2d3b3707e982dea906">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c1a58edb-1ba6-4800-9942-1e1defaa36d6" xmlns:ns3="4b113022-9134-4b2e-abe8-26e86c9e296e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="be9eaf82d0c074f79785b0acc776d2a9" ns2:_="" ns3:_="">
     <xsd:import namespace="c1a58edb-1ba6-4800-9942-1e1defaa36d6"/>
@@ -68209,36 +68203,26 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4A36FDD-FA0C-40EF-989B-74F1F7876F18}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="4b113022-9134-4b2e-abe8-26e86c9e296e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="c1a58edb-1ba6-4800-9942-1e1defaa36d6"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2D8D0BD-9993-4EC8-86D1-0A7C5F6E1934}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D3F3134-699E-462F-8D9F-EA7A8DE51B1D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -68257,6 +68241,31 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2D8D0BD-9993-4EC8-86D1-0A7C5F6E1934}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4A36FDD-FA0C-40EF-989B-74F1F7876F18}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="4b113022-9134-4b2e-abe8-26e86c9e296e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="c1a58edb-1ba6-4800-9942-1e1defaa36d6"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6E1C13E-614F-4B48-A9FE-F6158F0F568F}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
update script and xls
</commit_message>
<xml_diff>
--- a/input/images/IJE_File_Layouts_Version_2021_FHIR.xlsx
+++ b/input/images/IJE_File_Layouts_Version_2021_FHIR.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skravitz/git/vrdr/input/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F97F16F6-D5FB-4B43-86F6-EDC241DF111A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5B76C0A-708F-684D-85E1-D17C1495C3A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4000" yWindow="500" windowWidth="63620" windowHeight="27760" tabRatio="779" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -55,7 +55,7 @@
     <definedName name="Z_F1069C25_F3CC_400B_8C16_E88E31027CCC_.wvu.PrintTitles" localSheetId="4" hidden="1">Natality!$1:$8</definedName>
     <definedName name="Z_F1069C25_F3CC_400B_8C16_E88E31027CCC_.wvu.PrintTitles" localSheetId="2" hidden="1">Surveillance!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <customWorkbookViews>
     <customWorkbookView name="William Bolton - Personal View" guid="{F1069C25-F3CC-400B-8C16-E88E31027CCC}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1024" windowHeight="576" tabRatio="779" activeSheetId="1"/>
   </customWorkbookViews>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7734" uniqueCount="2695">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7734" uniqueCount="2696">
   <si>
     <t>u</t>
   </si>
@@ -9339,6 +9339,9 @@
   </si>
   <si>
     <t>12 digit number</t>
+  </si>
+  <si>
+    <t>a code from [PlaceOfInjuryVS] is required, an optional code from [PlaceOfInjuryOtherVS] can also be provided.</t>
   </si>
 </sst>
 </file>
@@ -11894,8 +11897,8 @@
   </sheetPr>
   <dimension ref="A1:L284"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E16" zoomScale="220" zoomScaleNormal="220" zoomScaleSheetLayoutView="95" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView tabSelected="1" topLeftCell="E105" zoomScale="220" zoomScaleNormal="220" zoomScaleSheetLayoutView="95" workbookViewId="0">
+      <selection activeCell="K121" sqref="K121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13"/>
@@ -16160,7 +16163,7 @@
         <v>2361</v>
       </c>
       <c r="K120" s="16" t="s">
-        <v>2616</v>
+        <v>2695</v>
       </c>
     </row>
     <row r="121" spans="1:12" ht="14">
@@ -68007,15 +68010,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002752A2C1F044FE469AAF2142AB326B8C" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c07487fc32f7ac2d3b3707e982dea906">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c1a58edb-1ba6-4800-9942-1e1defaa36d6" xmlns:ns3="4b113022-9134-4b2e-abe8-26e86c9e296e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="be9eaf82d0c074f79785b0acc776d2a9" ns2:_="" ns3:_="">
     <xsd:import namespace="c1a58edb-1ba6-4800-9942-1e1defaa36d6"/>
@@ -68218,25 +68212,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2D8D0BD-9993-4EC8-86D1-0A7C5F6E1934}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D3F3134-699E-462F-8D9F-EA7A8DE51B1D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -68255,15 +68250,15 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6E1C13E-614F-4B48-A9FE-F6158F0F568F}">
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2D8D0BD-9993-4EC8-86D1-0A7C5F6E1934}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4A36FDD-FA0C-40EF-989B-74F1F7876F18}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -68278,4 +68273,12 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6E1C13E-614F-4B48-A9FE-F6158F0F568F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>